<commit_message>
Fix examplecontent repositories, make sure initial content can be created.
</commit_message>
<xml_diff>
--- a/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/ordnungssystem.xlsx
+++ b/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/ordnungssystem.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="23460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ordnungssystem" sheetId="1" r:id="rId1"/>
     <sheet name="Wertebereich" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
     <definedName name="repository" localSheetId="0">Ordnungssystem!$A$7:$X$22</definedName>
   </definedNames>
@@ -58,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="241">
   <si>
     <t>reference_number</t>
   </si>
@@ -838,6 +841,27 @@
   </si>
   <si>
     <t>Kommission für Rechtsfragen</t>
+  </si>
+  <si>
+    <t>0.9.0</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>0.9.1</t>
+  </si>
+  <si>
+    <t>Planung und Organisatorisches</t>
+  </si>
+  <si>
+    <t>Kommunikation</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>0.10.0</t>
   </si>
 </sst>
 </file>
@@ -1271,6 +1295,21 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Ordnungssystem"/>
+      <sheetName val="Wertebereich"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="repository" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -1598,13 +1637,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blatt1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:W78"/>
+  <dimension ref="A1:W83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2525,19 +2564,30 @@
     </row>
     <row r="29" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A29" s="31" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="C29" s="21">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="D29" s="21">
+        <v>0</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K29" s="22"/>
+      <c r="J29" s="21">
+        <v>10</v>
+      </c>
+      <c r="K29" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="L29" s="28" t="s">
+        <v>40</v>
+      </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="25"/>
       <c r="S29" s="25"/>
@@ -2547,13 +2597,16 @@
     </row>
     <row r="30" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A30" s="31" t="s">
-        <v>179</v>
+        <v>236</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>120</v>
+        <v>237</v>
       </c>
       <c r="C30" s="21">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D30" s="21">
+        <v>1</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="26" t="s">
@@ -2569,13 +2622,13 @@
     </row>
     <row r="31" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A31" s="31" t="s">
-        <v>82</v>
+        <v>178</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="C31" s="21">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="26" t="s">
@@ -2591,13 +2644,13 @@
     </row>
     <row r="32" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A32" s="31" t="s">
-        <v>83</v>
+        <v>239</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>122</v>
+        <v>238</v>
       </c>
       <c r="C32" s="21">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="26" t="s">
@@ -2611,20 +2664,32 @@
       <c r="U32" s="25"/>
       <c r="V32" s="25"/>
     </row>
-    <row r="33" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="33" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A33" s="31" t="s">
-        <v>28</v>
+        <v>240</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>221</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C33" s="21">
+        <v>11</v>
+      </c>
+      <c r="D33" s="21">
+        <v>0</v>
+      </c>
+      <c r="F33" s="22"/>
       <c r="G33" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K33" s="22"/>
+      <c r="J33" s="21">
+        <v>10</v>
+      </c>
+      <c r="K33" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L33" s="28" t="s">
+        <v>40</v>
+      </c>
       <c r="Q33" s="25"/>
       <c r="R33" s="25"/>
       <c r="S33" s="25"/>
@@ -2634,10 +2699,13 @@
     </row>
     <row r="34" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A34" s="31" t="s">
-        <v>29</v>
+        <v>232</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>129</v>
+        <v>119</v>
+      </c>
+      <c r="C34" s="21">
+        <v>12</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="26" t="s">
@@ -2653,10 +2721,13 @@
     </row>
     <row r="35" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A35" s="31" t="s">
-        <v>30</v>
+        <v>179</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>130</v>
+        <v>120</v>
+      </c>
+      <c r="C35" s="21">
+        <v>0</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="26" t="s">
@@ -2672,10 +2743,13 @@
     </row>
     <row r="36" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A36" s="31" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>131</v>
+        <v>121</v>
+      </c>
+      <c r="C36" s="21">
+        <v>1</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="26" t="s">
@@ -2691,10 +2765,13 @@
     </row>
     <row r="37" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A37" s="31" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>132</v>
+        <v>122</v>
+      </c>
+      <c r="C37" s="21">
+        <v>2</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="26" t="s">
@@ -2708,14 +2785,16 @@
       <c r="U37" s="25"/>
       <c r="V37" s="25"/>
     </row>
-    <row r="38" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="38" spans="1:22" s="16" customFormat="1" ht="36">
       <c r="A38" s="31" t="s">
-        <v>180</v>
+        <v>28</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="F38" s="22"/>
+        <v>123</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>221</v>
+      </c>
       <c r="G38" s="26" t="s">
         <v>34</v>
       </c>
@@ -2729,10 +2808,10 @@
     </row>
     <row r="39" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A39" s="31" t="s">
-        <v>181</v>
+        <v>29</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="26" t="s">
@@ -2748,10 +2827,10 @@
     </row>
     <row r="40" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A40" s="31" t="s">
-        <v>182</v>
+        <v>30</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="26" t="s">
@@ -2767,13 +2846,10 @@
     </row>
     <row r="41" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A41" s="31" t="s">
-        <v>183</v>
+        <v>31</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="21">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="26" t="s">
@@ -2789,30 +2865,16 @@
     </row>
     <row r="42" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A42" s="31" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="21">
-        <v>0</v>
-      </c>
-      <c r="D42" s="21">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J42" s="21">
-        <v>10</v>
-      </c>
-      <c r="K42" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="L42" s="28" t="s">
-        <v>40</v>
-      </c>
+      <c r="K42" s="22"/>
       <c r="Q42" s="25"/>
       <c r="R42" s="25"/>
       <c r="S42" s="25"/>
@@ -2822,16 +2884,10 @@
     </row>
     <row r="43" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A43" s="31" t="s">
-        <v>137</v>
+        <v>180</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="C43" s="21">
-        <v>0</v>
-      </c>
-      <c r="D43" s="21">
-        <v>1</v>
+        <v>133</v>
       </c>
       <c r="F43" s="22"/>
       <c r="G43" s="26" t="s">
@@ -2845,33 +2901,18 @@
       <c r="U43" s="25"/>
       <c r="V43" s="25"/>
     </row>
-    <row r="44" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="44" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A44" s="31" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="C44" s="21">
-        <v>0</v>
-      </c>
-      <c r="D44" s="21">
-        <v>1</v>
-      </c>
-      <c r="E44" s="21"/>
+        <v>134</v>
+      </c>
       <c r="F44" s="22"/>
       <c r="G44" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J44" s="21">
-        <v>50</v>
-      </c>
-      <c r="K44" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="L44" s="28" t="s">
-        <v>40</v>
-      </c>
+      <c r="K44" s="22"/>
       <c r="Q44" s="25"/>
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
@@ -2881,31 +2922,16 @@
     </row>
     <row r="45" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A45" s="31" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="C45" s="21">
-        <v>0</v>
-      </c>
-      <c r="D45" s="21">
-        <v>1</v>
-      </c>
-      <c r="E45" s="21"/>
+        <v>135</v>
+      </c>
       <c r="F45" s="22"/>
       <c r="G45" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J45" s="21">
-        <v>10</v>
-      </c>
-      <c r="K45" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="L45" s="28" t="s">
-        <v>40</v>
-      </c>
+      <c r="K45" s="22"/>
       <c r="Q45" s="25"/>
       <c r="R45" s="25"/>
       <c r="S45" s="25"/>
@@ -2913,34 +2939,21 @@
       <c r="U45" s="25"/>
       <c r="V45" s="25"/>
     </row>
-    <row r="46" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="46" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A46" s="31" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C46" s="21">
         <v>0</v>
       </c>
-      <c r="D46" s="21">
-        <v>2</v>
-      </c>
-      <c r="F46" s="27" t="s">
-        <v>210</v>
-      </c>
+      <c r="F46" s="22"/>
       <c r="G46" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J46" s="21">
-        <v>50</v>
-      </c>
-      <c r="K46" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="L46" s="28" t="s">
-        <v>40</v>
-      </c>
+      <c r="K46" s="22"/>
       <c r="Q46" s="25"/>
       <c r="R46" s="25"/>
       <c r="S46" s="25"/>
@@ -2948,28 +2961,28 @@
       <c r="U46" s="25"/>
       <c r="V46" s="25"/>
     </row>
-    <row r="47" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="47" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A47" s="31" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C47" s="21">
         <v>0</v>
       </c>
       <c r="D47" s="21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F47" s="22"/>
       <c r="G47" s="26" t="s">
         <v>34</v>
       </c>
       <c r="J47" s="21">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="K47" s="27" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="L47" s="28" t="s">
         <v>40</v>
@@ -2983,16 +2996,16 @@
     </row>
     <row r="48" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A48" s="31" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C48" s="21">
         <v>0</v>
       </c>
       <c r="D48" s="21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F48" s="22"/>
       <c r="G48" s="26" t="s">
@@ -3006,24 +3019,33 @@
       <c r="U48" s="25"/>
       <c r="V48" s="25"/>
     </row>
-    <row r="49" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="49" spans="1:22" s="16" customFormat="1" ht="36">
       <c r="A49" s="31" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C49" s="21">
         <v>0</v>
       </c>
       <c r="D49" s="21">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E49" s="21"/>
       <c r="F49" s="22"/>
       <c r="G49" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K49" s="22"/>
+      <c r="J49" s="21">
+        <v>50</v>
+      </c>
+      <c r="K49" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="L49" s="28" t="s">
+        <v>40</v>
+      </c>
       <c r="Q49" s="25"/>
       <c r="R49" s="25"/>
       <c r="S49" s="25"/>
@@ -3031,19 +3053,20 @@
       <c r="U49" s="25"/>
       <c r="V49" s="25"/>
     </row>
-    <row r="50" spans="1:22" s="16" customFormat="1" ht="24">
+    <row r="50" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A50" s="31" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C50" s="21">
         <v>0</v>
       </c>
       <c r="D50" s="21">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E50" s="21"/>
       <c r="F50" s="22"/>
       <c r="G50" s="26" t="s">
         <v>34</v>
@@ -3052,10 +3075,10 @@
         <v>10</v>
       </c>
       <c r="K50" s="27" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L50" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q50" s="25"/>
       <c r="R50" s="25"/>
@@ -3064,33 +3087,33 @@
       <c r="U50" s="25"/>
       <c r="V50" s="25"/>
     </row>
-    <row r="51" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="51" spans="1:22" s="16" customFormat="1" ht="36">
       <c r="A51" s="31" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>152</v>
+        <v>21</v>
       </c>
       <c r="C51" s="21">
         <v>0</v>
       </c>
       <c r="D51" s="21">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F51" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G51" s="26" t="s">
         <v>34</v>
       </c>
       <c r="J51" s="21">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="K51" s="27" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="L51" s="28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q51" s="25"/>
       <c r="R51" s="25"/>
@@ -3099,28 +3122,28 @@
       <c r="U51" s="25"/>
       <c r="V51" s="25"/>
     </row>
-    <row r="52" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="52" spans="1:22" s="16" customFormat="1" ht="36">
       <c r="A52" s="31" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>154</v>
+        <v>86</v>
       </c>
       <c r="C52" s="21">
         <v>0</v>
       </c>
       <c r="D52" s="21">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="26" t="s">
         <v>34</v>
       </c>
       <c r="J52" s="21">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="K52" s="27" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="L52" s="28" t="s">
         <v>40</v>
@@ -3134,30 +3157,22 @@
     </row>
     <row r="53" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A53" s="31" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C53" s="21">
         <v>0</v>
       </c>
       <c r="D53" s="21">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J53" s="21">
-        <v>30</v>
-      </c>
-      <c r="K53" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="L53" s="28" t="s">
-        <v>42</v>
-      </c>
+      <c r="K53" s="22"/>
       <c r="Q53" s="25"/>
       <c r="R53" s="25"/>
       <c r="S53" s="25"/>
@@ -3167,13 +3182,16 @@
     </row>
     <row r="54" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A54" s="31" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C54" s="21">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D54" s="21">
+        <v>5</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="26" t="s">
@@ -3187,21 +3205,32 @@
       <c r="U54" s="25"/>
       <c r="V54" s="25"/>
     </row>
-    <row r="55" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="55" spans="1:22" s="16" customFormat="1" ht="24">
       <c r="A55" s="31" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="C55" s="21">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D55" s="21">
+        <v>6</v>
       </c>
       <c r="F55" s="22"/>
       <c r="G55" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K55" s="22"/>
+      <c r="J55" s="21">
+        <v>10</v>
+      </c>
+      <c r="K55" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="L55" s="28" t="s">
+        <v>41</v>
+      </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="25"/>
       <c r="S55" s="25"/>
@@ -3209,21 +3238,21 @@
       <c r="U55" s="25"/>
       <c r="V55" s="25"/>
     </row>
-    <row r="56" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="56" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A56" s="31" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="C56" s="21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D56" s="21">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F56" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G56" s="26" t="s">
         <v>34</v>
@@ -3232,10 +3261,10 @@
         <v>10</v>
       </c>
       <c r="K56" s="27" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L56" s="28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="Q56" s="25"/>
       <c r="R56" s="25"/>
@@ -3246,16 +3275,16 @@
     </row>
     <row r="57" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A57" s="31" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="C57" s="21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D57" s="21">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F57" s="22"/>
       <c r="G57" s="26" t="s">
@@ -3268,7 +3297,7 @@
         <v>226</v>
       </c>
       <c r="L57" s="28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q57" s="25"/>
       <c r="R57" s="25"/>
@@ -3279,22 +3308,30 @@
     </row>
     <row r="58" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A58" s="31" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="C58" s="21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D58" s="21">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F58" s="22"/>
       <c r="G58" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K58" s="22"/>
+      <c r="J58" s="21">
+        <v>30</v>
+      </c>
+      <c r="K58" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="L58" s="28" t="s">
+        <v>42</v>
+      </c>
       <c r="Q58" s="25"/>
       <c r="R58" s="25"/>
       <c r="S58" s="25"/>
@@ -3302,34 +3339,21 @@
       <c r="U58" s="25"/>
       <c r="V58" s="25"/>
     </row>
-    <row r="59" spans="1:22" s="16" customFormat="1" ht="24">
+    <row r="59" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A59" s="31" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="C59" s="21">
-        <v>2</v>
-      </c>
-      <c r="D59" s="21">
-        <v>3</v>
-      </c>
-      <c r="F59" s="27" t="s">
-        <v>209</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F59" s="22"/>
       <c r="G59" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J59" s="21">
-        <v>10</v>
-      </c>
-      <c r="K59" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="L59" s="28" t="s">
-        <v>42</v>
-      </c>
+      <c r="K59" s="22"/>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
       <c r="S59" s="25"/>
@@ -3337,34 +3361,21 @@
       <c r="U59" s="25"/>
       <c r="V59" s="25"/>
     </row>
-    <row r="60" spans="1:22" s="16" customFormat="1" ht="24">
+    <row r="60" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A60" s="31" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="C60" s="21">
         <v>2</v>
       </c>
-      <c r="D60" s="21">
-        <v>4</v>
-      </c>
-      <c r="F60" s="27" t="s">
-        <v>222</v>
-      </c>
+      <c r="F60" s="22"/>
       <c r="G60" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J60" s="21">
-        <v>10</v>
-      </c>
-      <c r="K60" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="L60" s="28" t="s">
-        <v>42</v>
-      </c>
+      <c r="K60" s="22"/>
       <c r="Q60" s="25"/>
       <c r="R60" s="25"/>
       <c r="S60" s="25"/>
@@ -3372,21 +3383,21 @@
       <c r="U60" s="25"/>
       <c r="V60" s="25"/>
     </row>
-    <row r="61" spans="1:22" s="16" customFormat="1" ht="24">
+    <row r="61" spans="1:22" s="16" customFormat="1" ht="36">
       <c r="A61" s="31" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="C61" s="21">
         <v>2</v>
       </c>
       <c r="D61" s="21">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F61" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G61" s="26" t="s">
         <v>34</v>
@@ -3398,7 +3409,7 @@
         <v>226</v>
       </c>
       <c r="L61" s="28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q61" s="25"/>
       <c r="R61" s="25"/>
@@ -3409,20 +3420,18 @@
     </row>
     <row r="62" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A62" s="31" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C62" s="21">
         <v>2</v>
       </c>
       <c r="D62" s="21">
-        <v>6</v>
-      </c>
-      <c r="F62" s="27" t="s">
-        <v>223</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F62" s="22"/>
       <c r="G62" s="26" t="s">
         <v>34</v>
       </c>
@@ -3442,34 +3451,24 @@
       <c r="U62" s="25"/>
       <c r="V62" s="25"/>
     </row>
-    <row r="63" spans="1:22" s="16" customFormat="1" ht="48">
+    <row r="63" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A63" s="31" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="C63" s="21">
         <v>2</v>
       </c>
       <c r="D63" s="21">
-        <v>7</v>
-      </c>
-      <c r="F63" s="27" t="s">
-        <v>224</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F63" s="22"/>
       <c r="G63" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J63" s="21">
-        <v>10</v>
-      </c>
-      <c r="K63" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="L63" s="28" t="s">
-        <v>42</v>
-      </c>
+      <c r="K63" s="22"/>
       <c r="Q63" s="25"/>
       <c r="R63" s="25"/>
       <c r="S63" s="25"/>
@@ -3477,20 +3476,22 @@
       <c r="U63" s="25"/>
       <c r="V63" s="25"/>
     </row>
-    <row r="64" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="64" spans="1:22" s="16" customFormat="1" ht="24">
       <c r="A64" s="31" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="C64" s="21">
         <v>2</v>
       </c>
       <c r="D64" s="21">
-        <v>8</v>
-      </c>
-      <c r="F64" s="22"/>
+        <v>3</v>
+      </c>
+      <c r="F64" s="27" t="s">
+        <v>209</v>
+      </c>
       <c r="G64" s="26" t="s">
         <v>34</v>
       </c>
@@ -3501,7 +3502,7 @@
         <v>226</v>
       </c>
       <c r="L64" s="28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q64" s="25"/>
       <c r="R64" s="25"/>
@@ -3510,21 +3511,21 @@
       <c r="U64" s="25"/>
       <c r="V64" s="25"/>
     </row>
-    <row r="65" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="65" spans="1:22" s="16" customFormat="1" ht="24">
       <c r="A65" s="31" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="C65" s="21">
         <v>2</v>
       </c>
       <c r="D65" s="21">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F65" s="27" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="G65" s="26" t="s">
         <v>34</v>
@@ -3533,10 +3534,10 @@
         <v>10</v>
       </c>
       <c r="K65" s="27" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="L65" s="28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q65" s="25"/>
       <c r="R65" s="25"/>
@@ -3545,24 +3546,34 @@
       <c r="U65" s="25"/>
       <c r="V65" s="25"/>
     </row>
-    <row r="66" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="66" spans="1:22" s="16" customFormat="1" ht="24">
       <c r="A66" s="31" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C66" s="21">
         <v>2</v>
       </c>
       <c r="D66" s="21">
+        <v>5</v>
+      </c>
+      <c r="F66" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="G66" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="J66" s="21">
         <v>10</v>
       </c>
-      <c r="F66" s="22"/>
-      <c r="G66" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="K66" s="22"/>
+      <c r="K66" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L66" s="28" t="s">
+        <v>42</v>
+      </c>
       <c r="Q66" s="25"/>
       <c r="R66" s="25"/>
       <c r="S66" s="25"/>
@@ -3572,22 +3583,32 @@
     </row>
     <row r="67" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A67" s="31" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="C67" s="21">
         <v>2</v>
       </c>
       <c r="D67" s="21">
-        <v>11</v>
-      </c>
-      <c r="F67" s="22"/>
+        <v>6</v>
+      </c>
+      <c r="F67" s="27" t="s">
+        <v>223</v>
+      </c>
       <c r="G67" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K67" s="22"/>
+      <c r="J67" s="21">
+        <v>10</v>
+      </c>
+      <c r="K67" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L67" s="28" t="s">
+        <v>42</v>
+      </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="25"/>
       <c r="S67" s="25"/>
@@ -3595,21 +3616,34 @@
       <c r="U67" s="25"/>
       <c r="V67" s="25"/>
     </row>
-    <row r="68" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="68" spans="1:22" s="16" customFormat="1" ht="48">
       <c r="A68" s="31" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C68" s="21">
-        <v>3</v>
-      </c>
-      <c r="F68" s="22"/>
+        <v>2</v>
+      </c>
+      <c r="D68" s="21">
+        <v>7</v>
+      </c>
+      <c r="F68" s="27" t="s">
+        <v>224</v>
+      </c>
       <c r="G68" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K68" s="22"/>
+      <c r="J68" s="21">
+        <v>10</v>
+      </c>
+      <c r="K68" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L68" s="28" t="s">
+        <v>42</v>
+      </c>
       <c r="Q68" s="25"/>
       <c r="R68" s="25"/>
       <c r="S68" s="25"/>
@@ -3619,19 +3653,30 @@
     </row>
     <row r="69" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A69" s="31" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C69" s="21">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D69" s="21">
+        <v>8</v>
       </c>
       <c r="F69" s="22"/>
       <c r="G69" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K69" s="22"/>
+      <c r="J69" s="21">
+        <v>10</v>
+      </c>
+      <c r="K69" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L69" s="28" t="s">
+        <v>41</v>
+      </c>
       <c r="Q69" s="25"/>
       <c r="R69" s="25"/>
       <c r="S69" s="25"/>
@@ -3641,18 +3686,20 @@
     </row>
     <row r="70" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A70" s="31" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
       <c r="C70" s="21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D70" s="21">
-        <v>0</v>
-      </c>
-      <c r="F70" s="22"/>
+        <v>9</v>
+      </c>
+      <c r="F70" s="27" t="s">
+        <v>214</v>
+      </c>
       <c r="G70" s="26" t="s">
         <v>34</v>
       </c>
@@ -3663,7 +3710,7 @@
         <v>226</v>
       </c>
       <c r="L70" s="28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q70" s="25"/>
       <c r="R70" s="25"/>
@@ -3674,32 +3721,22 @@
     </row>
     <row r="71" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A71" s="31" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="C71" s="21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D71" s="21">
-        <v>1</v>
-      </c>
-      <c r="F71" s="27" t="s">
-        <v>215</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F71" s="22"/>
       <c r="G71" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J71" s="21">
-        <v>10</v>
-      </c>
-      <c r="K71" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="L71" s="28" t="s">
-        <v>41</v>
-      </c>
+      <c r="K71" s="22"/>
       <c r="Q71" s="25"/>
       <c r="R71" s="25"/>
       <c r="S71" s="25"/>
@@ -3709,32 +3746,22 @@
     </row>
     <row r="72" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A72" s="31" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C72" s="21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D72" s="21">
-        <v>2</v>
-      </c>
-      <c r="F72" s="27" t="s">
-        <v>225</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F72" s="22"/>
       <c r="G72" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J72" s="21">
-        <v>10</v>
-      </c>
-      <c r="K72" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="L72" s="28" t="s">
-        <v>41</v>
-      </c>
+      <c r="K72" s="22"/>
       <c r="Q72" s="25"/>
       <c r="R72" s="25"/>
       <c r="S72" s="25"/>
@@ -3744,30 +3771,19 @@
     </row>
     <row r="73" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A73" s="31" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C73" s="21">
-        <v>4</v>
-      </c>
-      <c r="D73" s="21">
         <v>3</v>
       </c>
       <c r="F73" s="22"/>
       <c r="G73" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J73" s="21">
-        <v>10</v>
-      </c>
-      <c r="K73" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="L73" s="28" t="s">
-        <v>41</v>
-      </c>
+      <c r="K73" s="22"/>
       <c r="Q73" s="25"/>
       <c r="R73" s="25"/>
       <c r="S73" s="25"/>
@@ -3777,32 +3793,19 @@
     </row>
     <row r="74" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A74" s="31" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C74" s="21">
         <v>4</v>
       </c>
-      <c r="D74" s="21">
-        <v>4</v>
-      </c>
-      <c r="F74" s="27" t="s">
-        <v>216</v>
-      </c>
+      <c r="F74" s="22"/>
       <c r="G74" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J74" s="21">
-        <v>10</v>
-      </c>
-      <c r="K74" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="L74" s="28" t="s">
-        <v>41</v>
-      </c>
+      <c r="K74" s="22"/>
       <c r="Q74" s="25"/>
       <c r="R74" s="25"/>
       <c r="S74" s="25"/>
@@ -3812,19 +3815,30 @@
     </row>
     <row r="75" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A75" s="31" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B75" s="21" t="s">
-        <v>168</v>
+        <v>94</v>
       </c>
       <c r="C75" s="21">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D75" s="21">
+        <v>0</v>
       </c>
       <c r="F75" s="22"/>
       <c r="G75" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K75" s="22"/>
+      <c r="J75" s="21">
+        <v>10</v>
+      </c>
+      <c r="K75" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L75" s="28" t="s">
+        <v>40</v>
+      </c>
       <c r="Q75" s="25"/>
       <c r="R75" s="25"/>
       <c r="S75" s="25"/>
@@ -3834,18 +3848,20 @@
     </row>
     <row r="76" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A76" s="31" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C76" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D76" s="21">
-        <v>0</v>
-      </c>
-      <c r="F76" s="22"/>
+        <v>1</v>
+      </c>
+      <c r="F76" s="27" t="s">
+        <v>215</v>
+      </c>
       <c r="G76" s="26" t="s">
         <v>34</v>
       </c>
@@ -3856,7 +3872,7 @@
         <v>226</v>
       </c>
       <c r="L76" s="28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q76" s="25"/>
       <c r="R76" s="25"/>
@@ -3867,22 +3883,32 @@
     </row>
     <row r="77" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A77" s="31" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
       <c r="C77" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D77" s="21">
-        <v>1</v>
-      </c>
-      <c r="F77" s="22"/>
+        <v>2</v>
+      </c>
+      <c r="F77" s="27" t="s">
+        <v>225</v>
+      </c>
       <c r="G77" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K77" s="22"/>
+      <c r="J77" s="21">
+        <v>10</v>
+      </c>
+      <c r="K77" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L77" s="28" t="s">
+        <v>41</v>
+      </c>
       <c r="Q77" s="25"/>
       <c r="R77" s="25"/>
       <c r="S77" s="25"/>
@@ -3892,22 +3918,30 @@
     </row>
     <row r="78" spans="1:22" s="16" customFormat="1" ht="12">
       <c r="A78" s="31" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C78" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D78" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F78" s="22"/>
       <c r="G78" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K78" s="22"/>
+      <c r="J78" s="21">
+        <v>10</v>
+      </c>
+      <c r="K78" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L78" s="28" t="s">
+        <v>41</v>
+      </c>
       <c r="Q78" s="25"/>
       <c r="R78" s="25"/>
       <c r="S78" s="25"/>
@@ -3915,54 +3949,224 @@
       <c r="U78" s="25"/>
       <c r="V78" s="25"/>
     </row>
+    <row r="79" spans="1:22" s="16" customFormat="1" ht="12">
+      <c r="A79" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" s="21">
+        <v>4</v>
+      </c>
+      <c r="D79" s="21">
+        <v>4</v>
+      </c>
+      <c r="F79" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="G79" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="J79" s="21">
+        <v>10</v>
+      </c>
+      <c r="K79" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L79" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q79" s="25"/>
+      <c r="R79" s="25"/>
+      <c r="S79" s="25"/>
+      <c r="T79" s="25"/>
+      <c r="U79" s="25"/>
+      <c r="V79" s="25"/>
+    </row>
+    <row r="80" spans="1:22" s="16" customFormat="1" ht="12">
+      <c r="A80" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C80" s="21">
+        <v>5</v>
+      </c>
+      <c r="F80" s="22"/>
+      <c r="G80" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K80" s="22"/>
+      <c r="Q80" s="25"/>
+      <c r="R80" s="25"/>
+      <c r="S80" s="25"/>
+      <c r="T80" s="25"/>
+      <c r="U80" s="25"/>
+      <c r="V80" s="25"/>
+    </row>
+    <row r="81" spans="1:22" s="16" customFormat="1" ht="12">
+      <c r="A81" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="21">
+        <v>5</v>
+      </c>
+      <c r="D81" s="21">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22"/>
+      <c r="G81" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="J81" s="21">
+        <v>10</v>
+      </c>
+      <c r="K81" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="L81" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q81" s="25"/>
+      <c r="R81" s="25"/>
+      <c r="S81" s="25"/>
+      <c r="T81" s="25"/>
+      <c r="U81" s="25"/>
+      <c r="V81" s="25"/>
+    </row>
+    <row r="82" spans="1:22" s="16" customFormat="1" ht="12">
+      <c r="A82" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C82" s="21">
+        <v>5</v>
+      </c>
+      <c r="D82" s="21">
+        <v>1</v>
+      </c>
+      <c r="F82" s="22"/>
+      <c r="G82" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K82" s="22"/>
+      <c r="Q82" s="25"/>
+      <c r="R82" s="25"/>
+      <c r="S82" s="25"/>
+      <c r="T82" s="25"/>
+      <c r="U82" s="25"/>
+      <c r="V82" s="25"/>
+    </row>
+    <row r="83" spans="1:22" s="16" customFormat="1" ht="12">
+      <c r="A83" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C83" s="21">
+        <v>5</v>
+      </c>
+      <c r="D83" s="21">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22"/>
+      <c r="G83" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K83" s="22"/>
+      <c r="Q83" s="25"/>
+      <c r="R83" s="25"/>
+      <c r="S83" s="25"/>
+      <c r="T83" s="25"/>
+      <c r="U83" s="25"/>
+      <c r="V83" s="25"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="235" yWindow="427" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="235" yWindow="427" count="12">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Wertebereich!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H5 H8:H1048576</xm:sqref>
+          <xm:sqref>H5 H8:H27 H31 H34:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Wertebereich!$H$2:$H$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I5 I8:I1048576</xm:sqref>
+          <xm:sqref>I5 I8:I27 I31 I34:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Wertebereich!$P$2:$P$4</xm:f>
           </x14:formula1>
-          <xm:sqref>Q5 Q8:Q1048576</xm:sqref>
+          <xm:sqref>Q5 Q8:Q27 Q31 Q34:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Wertebereich!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G5 G8:G1048576</xm:sqref>
+          <xm:sqref>G5 G8:G27 G31 G34:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Wertebereich!$K$2:$K$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L5 L79:L1048576</xm:sqref>
+          <xm:sqref>L5 L84:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Wertebereich!$I$2:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>J5 J79:J1048576</xm:sqref>
+          <xm:sqref>J5 J84:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Wertebereich!$M$2:$M$4</xm:f>
           </x14:formula1>
-          <xm:sqref>N5 N8:N1048576</xm:sqref>
+          <xm:sqref>N5 N8:N27 N31 N34:N1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Wertebereich!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>N28:N30 N32:N33</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Wertebereich!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>G28:G30 G32:G33</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Wertebereich!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q28:Q30 Q32:Q33</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Wertebereich!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>I28:I30 I32:I33</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Wertebereich!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>H28:H30 H32:H33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add specific add and edit forms for each object which supports translated titles.
</commit_message>
<xml_diff>
--- a/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/ordnungssystem.xlsx
+++ b/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/ordnungssystem.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="23460" tabRatio="500"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="305">
   <si>
     <t>reference_number</t>
   </si>
@@ -863,12 +863,204 @@
   <si>
     <t>0.10.0</t>
   </si>
+  <si>
+    <t>Bases juridiques, séances des organes</t>
+  </si>
+  <si>
+    <t>Généralités</t>
+  </si>
+  <si>
+    <t>Lignes directrices, stratégie, programme de travail</t>
+  </si>
+  <si>
+    <t>Rapport annuel</t>
+  </si>
+  <si>
+    <t>Planification</t>
+  </si>
+  <si>
+    <t>Bases juridiques</t>
+  </si>
+  <si>
+    <t>Concordat du 29.10.1970 sur la coordination scolaire</t>
+  </si>
+  <si>
+    <t>Accord intercantonal du 14.6.2007 sur l'harmonisation de la scolarité obligatoire (concordat HarmoS)</t>
+  </si>
+  <si>
+    <t>Accord intercantonal du 25.10.2007 sur la collaboration dans le domaine de la pédagogie spécialisée</t>
+  </si>
+  <si>
+    <t>Accord intercantonal du 18.6.2009 sur l'harmonisation des régimes de bourses d'études</t>
+  </si>
+  <si>
+    <t>Organisation de la CDIP</t>
+  </si>
+  <si>
+    <t>Financement de l'éducation</t>
+  </si>
+  <si>
+    <t>Accord intercantonal universitaire (AIU) du 20.2.1997</t>
+  </si>
+  <si>
+    <t>Convention intercantonale du 13.12.2002 relative aux institutions sociales (CIIS)</t>
+  </si>
+  <si>
+    <t>Accord intercantonal du 12.6.2003 sur les hautes écoles spécialisées (AHES) à partir de 2005</t>
+  </si>
+  <si>
+    <t>Accord intercantonal du 27.8.1998 sur les écoles supérieures spécialisées (AESS)</t>
+  </si>
+  <si>
+    <t>Accord intercantonal du 20.2.2003 sur les écoles offrant des formations spécifiques aux élèves surdoués</t>
+  </si>
+  <si>
+    <t>Accord intercantonal du 22.6.2006 sur les contributions dans le domaine de la formation professionnelle initiale (accord sur les écoles professionnelles, AEPr)</t>
+  </si>
+  <si>
+    <t>Accord intercantonal du 22.3.2012 sur les contributions dans le domaine des écoles supérieures (AES)</t>
+  </si>
+  <si>
+    <t>Reconnaissance de diplômes</t>
+  </si>
+  <si>
+    <t>Accord intercantonal du 18.2.1993 sur la reconnaissance des diplômes de fin d'études</t>
+  </si>
+  <si>
+    <t>Règlements de reconnaissance Degré secondaire II</t>
+  </si>
+  <si>
+    <t>Diplômes d'enseignement</t>
+  </si>
+  <si>
+    <t>Reconnaissance des diplômes étrangers</t>
+  </si>
+  <si>
+    <t>Plans d'études cadres</t>
+  </si>
+  <si>
+    <t>Domaine des hautes écoles</t>
+  </si>
+  <si>
+    <t>Accord intercantonal du 20.6.2013 sur le domaine suisse des hautes écoles (concordat sur les hautes écoles)</t>
+  </si>
+  <si>
+    <t>Assemblée plénière</t>
+  </si>
+  <si>
+    <t>Séances</t>
+  </si>
+  <si>
+    <t>Comité</t>
+  </si>
+  <si>
+    <t>Décisions par voie de correspondance</t>
+  </si>
+  <si>
+    <t>Commission des secrétaires généraux (CSG)</t>
+  </si>
+  <si>
+    <t>Conférence des secrétaires généraux (CSSG)</t>
+  </si>
+  <si>
+    <t>Administration du Secrétariat général</t>
+  </si>
+  <si>
+    <t>Fonctionnement</t>
+  </si>
+  <si>
+    <t>Archivage</t>
+  </si>
+  <si>
+    <t>Organisation du Secrétariat général</t>
+  </si>
+  <si>
+    <t>Processus / Aides-mémoires</t>
+  </si>
+  <si>
+    <t>Conseil de direction</t>
+  </si>
+  <si>
+    <t>Réunion des collaboratrices et collaborateurs / Forums</t>
+  </si>
+  <si>
+    <t>Appareils / Mobilier / Inventaire / Assurances choses</t>
+  </si>
+  <si>
+    <t>Locaux</t>
+  </si>
+  <si>
+    <t>Poste / Télécommunication</t>
+  </si>
+  <si>
+    <t>Informatique</t>
+  </si>
+  <si>
+    <t>Administration cantonale bernoise</t>
+  </si>
+  <si>
+    <t>Personnel</t>
+  </si>
+  <si>
+    <t>Mises au concours</t>
+  </si>
+  <si>
+    <t>Postulations</t>
+  </si>
+  <si>
+    <t>Dossiers du personnel</t>
+  </si>
+  <si>
+    <t>Office du personnel</t>
+  </si>
+  <si>
+    <t>Questions de salaire</t>
+  </si>
+  <si>
+    <t>Assurances sociales</t>
+  </si>
+  <si>
+    <t>Formation continue</t>
+  </si>
+  <si>
+    <t>Comptabilité</t>
+  </si>
+  <si>
+    <t>Généralités (plan comptable / indemnités et défraiements)</t>
+  </si>
+  <si>
+    <t>Contributions cantonales</t>
+  </si>
+  <si>
+    <t>Etat de comptes intermédiaire</t>
+  </si>
+  <si>
+    <t>Comptes annuels</t>
+  </si>
+  <si>
+    <t>Controlling</t>
+  </si>
+  <si>
+    <t>Subventions</t>
+  </si>
+  <si>
+    <t>Banque / Poste</t>
+  </si>
+  <si>
+    <t>Taxe sur la valeur ajoutée</t>
+  </si>
+  <si>
+    <t>Divers</t>
+  </si>
+  <si>
+    <t>Le Savoir du SG CDIP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -967,6 +1159,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1124,7 +1323,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1207,6 +1406,9 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="80">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1637,13 +1839,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blatt1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:W83"/>
+  <dimension ref="A1:W139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1923,12 +2125,15 @@
       <c r="T6" s="33"/>
       <c r="U6" s="33"/>
     </row>
-    <row r="7" spans="1:23" s="16" customFormat="1" ht="12">
+    <row r="7" spans="1:23" s="16" customFormat="1" ht="14">
       <c r="A7" s="32" t="s">
         <v>231</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>81</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>241</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
@@ -1946,7 +2151,7 @@
       <c r="U7" s="25"/>
       <c r="V7" s="25"/>
     </row>
-    <row r="8" spans="1:23" s="16" customFormat="1" ht="12">
+    <row r="8" spans="1:23" s="16" customFormat="1" ht="14">
       <c r="A8" s="31" t="s">
         <v>91</v>
       </c>
@@ -1955,6 +2160,9 @@
       </c>
       <c r="C8" s="21">
         <v>0</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>242</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="26" t="s">
@@ -1970,7 +2178,7 @@
       <c r="U8" s="25"/>
       <c r="V8" s="25"/>
     </row>
-    <row r="9" spans="1:23" s="16" customFormat="1" ht="12">
+    <row r="9" spans="1:23" s="16" customFormat="1" ht="14">
       <c r="A9" s="31" t="s">
         <v>170</v>
       </c>
@@ -1979,6 +2187,9 @@
       </c>
       <c r="C9" s="21">
         <v>1</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>243</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="26" t="s">
@@ -1994,7 +2205,7 @@
       <c r="U9" s="25"/>
       <c r="V9" s="25"/>
     </row>
-    <row r="10" spans="1:23" s="16" customFormat="1" ht="12">
+    <row r="10" spans="1:23" s="16" customFormat="1" ht="14">
       <c r="A10" s="31" t="s">
         <v>171</v>
       </c>
@@ -2003,6 +2214,9 @@
       </c>
       <c r="C10" s="21">
         <v>2</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>244</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="26" t="s">
@@ -2018,7 +2232,7 @@
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
     </row>
-    <row r="11" spans="1:23" s="16" customFormat="1" ht="12">
+    <row r="11" spans="1:23" s="16" customFormat="1" ht="14">
       <c r="A11" s="31" t="s">
         <v>172</v>
       </c>
@@ -2027,6 +2241,9 @@
       </c>
       <c r="C11" s="21">
         <v>3</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>245</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="26" t="s">
@@ -2042,7 +2259,7 @@
       <c r="U11" s="25"/>
       <c r="V11" s="25"/>
     </row>
-    <row r="12" spans="1:23" s="16" customFormat="1" ht="12">
+    <row r="12" spans="1:23" s="16" customFormat="1" ht="14">
       <c r="A12" s="31" t="s">
         <v>173</v>
       </c>
@@ -2051,6 +2268,9 @@
       </c>
       <c r="C12" s="21">
         <v>4</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>246</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="26" t="s">
@@ -2066,7 +2286,7 @@
       <c r="U12" s="25"/>
       <c r="V12" s="25"/>
     </row>
-    <row r="13" spans="1:23" s="16" customFormat="1" ht="36">
+    <row r="13" spans="1:23" s="16" customFormat="1" ht="37">
       <c r="A13" s="31" t="s">
         <v>174</v>
       </c>
@@ -2075,6 +2295,9 @@
       </c>
       <c r="C13" s="21">
         <v>5</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>242</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>217</v>
@@ -2092,7 +2315,7 @@
       <c r="U13" s="25"/>
       <c r="V13" s="25"/>
     </row>
-    <row r="14" spans="1:23" s="16" customFormat="1" ht="24">
+    <row r="14" spans="1:23" s="16" customFormat="1" ht="25">
       <c r="A14" s="31" t="s">
         <v>99</v>
       </c>
@@ -2104,6 +2327,9 @@
       </c>
       <c r="D14" s="21">
         <v>0</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>247</v>
       </c>
       <c r="F14" s="27" t="s">
         <v>218</v>
@@ -2129,7 +2355,7 @@
       <c r="U14" s="25"/>
       <c r="V14" s="25"/>
     </row>
-    <row r="15" spans="1:23" s="16" customFormat="1" ht="12">
+    <row r="15" spans="1:23" s="16" customFormat="1" ht="28">
       <c r="A15" s="31" t="s">
         <v>100</v>
       </c>
@@ -2141,6 +2367,9 @@
       </c>
       <c r="D15" s="21">
         <v>1</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>248</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="26" t="s">
@@ -2164,7 +2393,7 @@
       <c r="U15" s="25"/>
       <c r="V15" s="25"/>
     </row>
-    <row r="16" spans="1:23" s="16" customFormat="1" ht="12">
+    <row r="16" spans="1:23" s="16" customFormat="1" ht="28">
       <c r="A16" s="31" t="s">
         <v>102</v>
       </c>
@@ -2176,6 +2405,9 @@
       </c>
       <c r="D16" s="21">
         <v>2</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>249</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="26" t="s">
@@ -2199,7 +2431,7 @@
       <c r="U16" s="25"/>
       <c r="V16" s="25"/>
     </row>
-    <row r="17" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="17" spans="1:22" s="16" customFormat="1" ht="37">
       <c r="A17" s="31" t="s">
         <v>175</v>
       </c>
@@ -2208,6 +2440,9 @@
       </c>
       <c r="C17" s="21">
         <v>6</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>250</v>
       </c>
       <c r="F17" s="30" t="s">
         <v>219</v>
@@ -2225,7 +2460,7 @@
       <c r="U17" s="25"/>
       <c r="V17" s="25"/>
     </row>
-    <row r="18" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="18" spans="1:22" s="16" customFormat="1" ht="37">
       <c r="A18" s="31" t="s">
         <v>176</v>
       </c>
@@ -2234,6 +2469,9 @@
       </c>
       <c r="C18" s="21">
         <v>7</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>251</v>
       </c>
       <c r="F18" s="30" t="s">
         <v>220</v>
@@ -2252,7 +2490,7 @@
       <c r="U18" s="25"/>
       <c r="V18" s="25"/>
     </row>
-    <row r="19" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="19" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A19" s="31" t="s">
         <v>107</v>
       </c>
@@ -2264,6 +2502,9 @@
       </c>
       <c r="D19" s="21">
         <v>1</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>252</v>
       </c>
       <c r="F19" s="22"/>
       <c r="G19" s="26" t="s">
@@ -2280,7 +2521,7 @@
       <c r="U19" s="25"/>
       <c r="V19" s="25"/>
     </row>
-    <row r="20" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="20" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A20" s="31" t="s">
         <v>108</v>
       </c>
@@ -2293,7 +2534,9 @@
       <c r="D20" s="21">
         <v>1</v>
       </c>
-      <c r="E20" s="21"/>
+      <c r="E20" s="40" t="s">
+        <v>253</v>
+      </c>
       <c r="F20" s="22"/>
       <c r="G20" s="26" t="s">
         <v>34</v>
@@ -2317,7 +2560,7 @@
       <c r="U20" s="25"/>
       <c r="V20" s="25"/>
     </row>
-    <row r="21" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="21" spans="1:22" s="16" customFormat="1" ht="28">
       <c r="A21" s="31" t="s">
         <v>109</v>
       </c>
@@ -2330,7 +2573,9 @@
       <c r="D21" s="21">
         <v>1</v>
       </c>
-      <c r="E21" s="21"/>
+      <c r="E21" s="40" t="s">
+        <v>254</v>
+      </c>
       <c r="F21" s="22"/>
       <c r="G21" s="26" t="s">
         <v>34</v>
@@ -2354,7 +2599,7 @@
       <c r="U21" s="25"/>
       <c r="V21" s="25"/>
     </row>
-    <row r="22" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="22" spans="1:22" s="16" customFormat="1" ht="28">
       <c r="A22" s="31" t="s">
         <v>110</v>
       </c>
@@ -2367,7 +2612,9 @@
       <c r="D22" s="21">
         <v>1</v>
       </c>
-      <c r="E22" s="21"/>
+      <c r="E22" s="40" t="s">
+        <v>255</v>
+      </c>
       <c r="F22" s="22"/>
       <c r="G22" s="26" t="s">
         <v>34</v>
@@ -2391,7 +2638,7 @@
       <c r="U22" s="25"/>
       <c r="V22" s="25"/>
     </row>
-    <row r="23" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="23" spans="1:22" s="16" customFormat="1" ht="28">
       <c r="A23" s="31" t="s">
         <v>112</v>
       </c>
@@ -2403,6 +2650,9 @@
       </c>
       <c r="D23" s="21">
         <v>8</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>256</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="26" t="s">
@@ -2416,7 +2666,7 @@
       <c r="U23" s="25"/>
       <c r="V23" s="25"/>
     </row>
-    <row r="24" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="24" spans="1:22" s="16" customFormat="1" ht="28">
       <c r="A24" s="31" t="s">
         <v>113</v>
       </c>
@@ -2429,7 +2679,9 @@
       <c r="D24" s="21">
         <v>8</v>
       </c>
-      <c r="E24" s="21"/>
+      <c r="E24" s="40" t="s">
+        <v>257</v>
+      </c>
       <c r="F24" s="22"/>
       <c r="G24" s="26" t="s">
         <v>34</v>
@@ -2450,7 +2702,7 @@
       <c r="U24" s="25"/>
       <c r="V24" s="25"/>
     </row>
-    <row r="25" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="25" spans="1:22" s="16" customFormat="1" ht="42">
       <c r="A25" s="31" t="s">
         <v>114</v>
       </c>
@@ -2463,7 +2715,9 @@
       <c r="D25" s="21">
         <v>8</v>
       </c>
-      <c r="E25" s="21"/>
+      <c r="E25" s="40" t="s">
+        <v>258</v>
+      </c>
       <c r="F25" s="22"/>
       <c r="G25" s="26" t="s">
         <v>34</v>
@@ -2484,7 +2738,7 @@
       <c r="U25" s="25"/>
       <c r="V25" s="25"/>
     </row>
-    <row r="26" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="26" spans="1:22" s="16" customFormat="1" ht="28">
       <c r="A26" s="31" t="s">
         <v>115</v>
       </c>
@@ -2497,7 +2751,9 @@
       <c r="D26" s="21">
         <v>8</v>
       </c>
-      <c r="E26" s="21"/>
+      <c r="E26" s="40" t="s">
+        <v>259</v>
+      </c>
       <c r="F26" s="22"/>
       <c r="G26" s="26" t="s">
         <v>34</v>
@@ -2518,7 +2774,7 @@
       <c r="U26" s="25"/>
       <c r="V26" s="25"/>
     </row>
-    <row r="27" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="27" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A27" s="31" t="s">
         <v>177</v>
       </c>
@@ -2527,6 +2783,9 @@
       </c>
       <c r="C27" s="21">
         <v>8</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>260</v>
       </c>
       <c r="F27" s="22"/>
       <c r="G27" s="26" t="s">
@@ -2540,7 +2799,7 @@
       <c r="U27" s="25"/>
       <c r="V27" s="25"/>
     </row>
-    <row r="28" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="28" spans="1:22" s="16" customFormat="1" ht="28">
       <c r="A28" s="31" t="s">
         <v>178</v>
       </c>
@@ -2549,6 +2808,9 @@
       </c>
       <c r="C28" s="21">
         <v>9</v>
+      </c>
+      <c r="E28" s="40" t="s">
+        <v>261</v>
       </c>
       <c r="F28" s="22"/>
       <c r="G28" s="26" t="s">
@@ -2562,7 +2824,7 @@
       <c r="U28" s="25"/>
       <c r="V28" s="25"/>
     </row>
-    <row r="29" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="29" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A29" s="31" t="s">
         <v>234</v>
       </c>
@@ -2574,6 +2836,9 @@
       </c>
       <c r="D29" s="21">
         <v>0</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>242</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="26" t="s">
@@ -2595,7 +2860,7 @@
       <c r="U29" s="25"/>
       <c r="V29" s="25"/>
     </row>
-    <row r="30" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="30" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A30" s="31" t="s">
         <v>236</v>
       </c>
@@ -2607,6 +2872,9 @@
       </c>
       <c r="D30" s="21">
         <v>1</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>262</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="26" t="s">
@@ -2620,7 +2888,7 @@
       <c r="U30" s="25"/>
       <c r="V30" s="25"/>
     </row>
-    <row r="31" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="31" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A31" s="31" t="s">
         <v>178</v>
       </c>
@@ -2629,6 +2897,9 @@
       </c>
       <c r="C31" s="21">
         <v>9</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>263</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="26" t="s">
@@ -2642,7 +2913,7 @@
       <c r="U31" s="25"/>
       <c r="V31" s="25"/>
     </row>
-    <row r="32" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="32" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A32" s="31" t="s">
         <v>239</v>
       </c>
@@ -2651,6 +2922,9 @@
       </c>
       <c r="C32" s="21">
         <v>11</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>264</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="26" t="s">
@@ -2664,7 +2938,7 @@
       <c r="U32" s="25"/>
       <c r="V32" s="25"/>
     </row>
-    <row r="33" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="33" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A33" s="31" t="s">
         <v>240</v>
       </c>
@@ -2676,6 +2950,9 @@
       </c>
       <c r="D33" s="21">
         <v>0</v>
+      </c>
+      <c r="E33" s="40" t="s">
+        <v>265</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="26" t="s">
@@ -2697,7 +2974,7 @@
       <c r="U33" s="25"/>
       <c r="V33" s="25"/>
     </row>
-    <row r="34" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="34" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A34" s="31" t="s">
         <v>232</v>
       </c>
@@ -2706,6 +2983,9 @@
       </c>
       <c r="C34" s="21">
         <v>12</v>
+      </c>
+      <c r="E34" s="40" t="s">
+        <v>266</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="26" t="s">
@@ -2719,7 +2999,7 @@
       <c r="U34" s="25"/>
       <c r="V34" s="25"/>
     </row>
-    <row r="35" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="35" spans="1:22" s="16" customFormat="1" ht="28">
       <c r="A35" s="31" t="s">
         <v>179</v>
       </c>
@@ -2728,6 +3008,9 @@
       </c>
       <c r="C35" s="21">
         <v>0</v>
+      </c>
+      <c r="E35" s="40" t="s">
+        <v>267</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="26" t="s">
@@ -2741,7 +3024,7 @@
       <c r="U35" s="25"/>
       <c r="V35" s="25"/>
     </row>
-    <row r="36" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="36" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A36" s="31" t="s">
         <v>82</v>
       </c>
@@ -2750,6 +3033,9 @@
       </c>
       <c r="C36" s="21">
         <v>1</v>
+      </c>
+      <c r="E36" s="40" t="s">
+        <v>268</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="26" t="s">
@@ -2763,7 +3049,7 @@
       <c r="U36" s="25"/>
       <c r="V36" s="25"/>
     </row>
-    <row r="37" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="37" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A37" s="31" t="s">
         <v>83</v>
       </c>
@@ -2772,6 +3058,9 @@
       </c>
       <c r="C37" s="21">
         <v>2</v>
+      </c>
+      <c r="E37" s="40" t="s">
+        <v>242</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="26" t="s">
@@ -2785,12 +3074,15 @@
       <c r="U37" s="25"/>
       <c r="V37" s="25"/>
     </row>
-    <row r="38" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="38" spans="1:22" s="16" customFormat="1" ht="37">
       <c r="A38" s="31" t="s">
         <v>28</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>123</v>
+      </c>
+      <c r="E38" s="40" t="s">
+        <v>269</v>
       </c>
       <c r="F38" s="27" t="s">
         <v>221</v>
@@ -2806,12 +3098,15 @@
       <c r="U38" s="25"/>
       <c r="V38" s="25"/>
     </row>
-    <row r="39" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="39" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A39" s="31" t="s">
         <v>29</v>
       </c>
       <c r="B39" s="21" t="s">
         <v>129</v>
+      </c>
+      <c r="E39" s="40" t="s">
+        <v>270</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="26" t="s">
@@ -2825,12 +3120,15 @@
       <c r="U39" s="25"/>
       <c r="V39" s="25"/>
     </row>
-    <row r="40" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="40" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A40" s="31" t="s">
         <v>30</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>130</v>
+      </c>
+      <c r="E40" s="40" t="s">
+        <v>242</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="26" t="s">
@@ -2844,12 +3142,15 @@
       <c r="U40" s="25"/>
       <c r="V40" s="25"/>
     </row>
-    <row r="41" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="41" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A41" s="31" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="21" t="s">
         <v>131</v>
+      </c>
+      <c r="E41" s="40" t="s">
+        <v>269</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="26" t="s">
@@ -2863,12 +3164,15 @@
       <c r="U41" s="25"/>
       <c r="V41" s="25"/>
     </row>
-    <row r="42" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="42" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A42" s="31" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>132</v>
+      </c>
+      <c r="E42" s="40" t="s">
+        <v>271</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="26" t="s">
@@ -2882,12 +3186,15 @@
       <c r="U42" s="25"/>
       <c r="V42" s="25"/>
     </row>
-    <row r="43" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="43" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A43" s="31" t="s">
         <v>180</v>
       </c>
       <c r="B43" s="21" t="s">
         <v>133</v>
+      </c>
+      <c r="E43" s="40" t="s">
+        <v>272</v>
       </c>
       <c r="F43" s="22"/>
       <c r="G43" s="26" t="s">
@@ -2901,12 +3208,15 @@
       <c r="U43" s="25"/>
       <c r="V43" s="25"/>
     </row>
-    <row r="44" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="44" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A44" s="31" t="s">
         <v>181</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>134</v>
+      </c>
+      <c r="E44" s="40" t="s">
+        <v>242</v>
       </c>
       <c r="F44" s="22"/>
       <c r="G44" s="26" t="s">
@@ -2920,12 +3230,15 @@
       <c r="U44" s="25"/>
       <c r="V44" s="25"/>
     </row>
-    <row r="45" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="45" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A45" s="31" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>135</v>
+      </c>
+      <c r="E45" s="40" t="s">
+        <v>269</v>
       </c>
       <c r="F45" s="22"/>
       <c r="G45" s="26" t="s">
@@ -2939,7 +3252,7 @@
       <c r="U45" s="25"/>
       <c r="V45" s="25"/>
     </row>
-    <row r="46" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="46" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A46" s="31" t="s">
         <v>183</v>
       </c>
@@ -2948,6 +3261,9 @@
       </c>
       <c r="C46" s="21">
         <v>0</v>
+      </c>
+      <c r="E46" s="40" t="s">
+        <v>273</v>
       </c>
       <c r="F46" s="22"/>
       <c r="G46" s="26" t="s">
@@ -2961,7 +3277,7 @@
       <c r="U46" s="25"/>
       <c r="V46" s="25"/>
     </row>
-    <row r="47" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="47" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A47" s="31" t="s">
         <v>136</v>
       </c>
@@ -2973,6 +3289,9 @@
       </c>
       <c r="D47" s="21">
         <v>0</v>
+      </c>
+      <c r="E47" s="40" t="s">
+        <v>242</v>
       </c>
       <c r="F47" s="22"/>
       <c r="G47" s="26" t="s">
@@ -2994,7 +3313,7 @@
       <c r="U47" s="25"/>
       <c r="V47" s="25"/>
     </row>
-    <row r="48" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="48" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A48" s="31" t="s">
         <v>137</v>
       </c>
@@ -3006,6 +3325,9 @@
       </c>
       <c r="D48" s="21">
         <v>1</v>
+      </c>
+      <c r="E48" s="40" t="s">
+        <v>269</v>
       </c>
       <c r="F48" s="22"/>
       <c r="G48" s="26" t="s">
@@ -3019,7 +3341,7 @@
       <c r="U48" s="25"/>
       <c r="V48" s="25"/>
     </row>
-    <row r="49" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="49" spans="1:22" s="16" customFormat="1" ht="37">
       <c r="A49" s="31" t="s">
         <v>139</v>
       </c>
@@ -3032,7 +3354,9 @@
       <c r="D49" s="21">
         <v>1</v>
       </c>
-      <c r="E49" s="21"/>
+      <c r="E49" s="40" t="s">
+        <v>274</v>
+      </c>
       <c r="F49" s="22"/>
       <c r="G49" s="26" t="s">
         <v>34</v>
@@ -3053,7 +3377,7 @@
       <c r="U49" s="25"/>
       <c r="V49" s="25"/>
     </row>
-    <row r="50" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="50" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A50" s="31" t="s">
         <v>141</v>
       </c>
@@ -3066,7 +3390,9 @@
       <c r="D50" s="21">
         <v>1</v>
       </c>
-      <c r="E50" s="21"/>
+      <c r="E50" s="40" t="s">
+        <v>242</v>
+      </c>
       <c r="F50" s="22"/>
       <c r="G50" s="26" t="s">
         <v>34</v>
@@ -3087,7 +3413,7 @@
       <c r="U50" s="25"/>
       <c r="V50" s="25"/>
     </row>
-    <row r="51" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="51" spans="1:22" s="16" customFormat="1" ht="37">
       <c r="A51" s="31" t="s">
         <v>143</v>
       </c>
@@ -3099,6 +3425,9 @@
       </c>
       <c r="D51" s="21">
         <v>2</v>
+      </c>
+      <c r="E51" s="40" t="s">
+        <v>275</v>
       </c>
       <c r="F51" s="27" t="s">
         <v>210</v>
@@ -3122,7 +3451,7 @@
       <c r="U51" s="25"/>
       <c r="V51" s="25"/>
     </row>
-    <row r="52" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="52" spans="1:22" s="16" customFormat="1" ht="37">
       <c r="A52" s="31" t="s">
         <v>144</v>
       </c>
@@ -3134,6 +3463,9 @@
       </c>
       <c r="D52" s="21">
         <v>3</v>
+      </c>
+      <c r="E52" s="40" t="s">
+        <v>242</v>
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="26" t="s">
@@ -3155,7 +3487,7 @@
       <c r="U52" s="25"/>
       <c r="V52" s="25"/>
     </row>
-    <row r="53" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="53" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A53" s="31" t="s">
         <v>145</v>
       </c>
@@ -3167,6 +3499,9 @@
       </c>
       <c r="D53" s="21">
         <v>4</v>
+      </c>
+      <c r="E53" s="40" t="s">
+        <v>276</v>
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="26" t="s">
@@ -3180,7 +3515,7 @@
       <c r="U53" s="25"/>
       <c r="V53" s="25"/>
     </row>
-    <row r="54" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="54" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A54" s="31" t="s">
         <v>147</v>
       </c>
@@ -3192,6 +3527,9 @@
       </c>
       <c r="D54" s="21">
         <v>5</v>
+      </c>
+      <c r="E54" s="40" t="s">
+        <v>277</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="26" t="s">
@@ -3205,7 +3543,7 @@
       <c r="U54" s="25"/>
       <c r="V54" s="25"/>
     </row>
-    <row r="55" spans="1:22" s="16" customFormat="1" ht="24">
+    <row r="55" spans="1:22" s="16" customFormat="1" ht="25">
       <c r="A55" s="31" t="s">
         <v>149</v>
       </c>
@@ -3217,6 +3555,9 @@
       </c>
       <c r="D55" s="21">
         <v>6</v>
+      </c>
+      <c r="E55" s="40" t="s">
+        <v>278</v>
       </c>
       <c r="F55" s="22"/>
       <c r="G55" s="26" t="s">
@@ -3238,7 +3579,7 @@
       <c r="U55" s="25"/>
       <c r="V55" s="25"/>
     </row>
-    <row r="56" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="56" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A56" s="31" t="s">
         <v>151</v>
       </c>
@@ -3250,6 +3591,9 @@
       </c>
       <c r="D56" s="21">
         <v>7</v>
+      </c>
+      <c r="E56" s="40" t="s">
+        <v>279</v>
       </c>
       <c r="F56" s="27" t="s">
         <v>211</v>
@@ -3273,7 +3617,7 @@
       <c r="U56" s="25"/>
       <c r="V56" s="25"/>
     </row>
-    <row r="57" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="57" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A57" s="31" t="s">
         <v>153</v>
       </c>
@@ -3285,6 +3629,9 @@
       </c>
       <c r="D57" s="21">
         <v>8</v>
+      </c>
+      <c r="E57" s="40" t="s">
+        <v>280</v>
       </c>
       <c r="F57" s="22"/>
       <c r="G57" s="26" t="s">
@@ -3306,7 +3653,7 @@
       <c r="U57" s="25"/>
       <c r="V57" s="25"/>
     </row>
-    <row r="58" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="58" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A58" s="31" t="s">
         <v>155</v>
       </c>
@@ -3318,6 +3665,9 @@
       </c>
       <c r="D58" s="21">
         <v>9</v>
+      </c>
+      <c r="E58" s="40" t="s">
+        <v>281</v>
       </c>
       <c r="F58" s="22"/>
       <c r="G58" s="26" t="s">
@@ -3339,7 +3689,7 @@
       <c r="U58" s="25"/>
       <c r="V58" s="25"/>
     </row>
-    <row r="59" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="59" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A59" s="31" t="s">
         <v>184</v>
       </c>
@@ -3348,6 +3698,9 @@
       </c>
       <c r="C59" s="21">
         <v>1</v>
+      </c>
+      <c r="E59" s="40" t="s">
+        <v>282</v>
       </c>
       <c r="F59" s="22"/>
       <c r="G59" s="26" t="s">
@@ -3361,7 +3714,7 @@
       <c r="U59" s="25"/>
       <c r="V59" s="25"/>
     </row>
-    <row r="60" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="60" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A60" s="31" t="s">
         <v>185</v>
       </c>
@@ -3370,6 +3723,9 @@
       </c>
       <c r="C60" s="21">
         <v>2</v>
+      </c>
+      <c r="E60" s="40" t="s">
+        <v>283</v>
       </c>
       <c r="F60" s="22"/>
       <c r="G60" s="26" t="s">
@@ -3383,7 +3739,7 @@
       <c r="U60" s="25"/>
       <c r="V60" s="25"/>
     </row>
-    <row r="61" spans="1:22" s="16" customFormat="1" ht="36">
+    <row r="61" spans="1:22" s="16" customFormat="1" ht="37">
       <c r="A61" s="31" t="s">
         <v>186</v>
       </c>
@@ -3395,6 +3751,9 @@
       </c>
       <c r="D61" s="21">
         <v>0</v>
+      </c>
+      <c r="E61" s="40" t="s">
+        <v>284</v>
       </c>
       <c r="F61" s="27" t="s">
         <v>212</v>
@@ -3418,7 +3777,7 @@
       <c r="U61" s="25"/>
       <c r="V61" s="25"/>
     </row>
-    <row r="62" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="62" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A62" s="31" t="s">
         <v>187</v>
       </c>
@@ -3430,6 +3789,9 @@
       </c>
       <c r="D62" s="21">
         <v>1</v>
+      </c>
+      <c r="E62" s="40" t="s">
+        <v>285</v>
       </c>
       <c r="F62" s="22"/>
       <c r="G62" s="26" t="s">
@@ -3451,7 +3813,7 @@
       <c r="U62" s="25"/>
       <c r="V62" s="25"/>
     </row>
-    <row r="63" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="63" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A63" s="31" t="s">
         <v>188</v>
       </c>
@@ -3463,6 +3825,9 @@
       </c>
       <c r="D63" s="21">
         <v>2</v>
+      </c>
+      <c r="E63" s="40" t="s">
+        <v>286</v>
       </c>
       <c r="F63" s="22"/>
       <c r="G63" s="26" t="s">
@@ -3476,7 +3841,7 @@
       <c r="U63" s="25"/>
       <c r="V63" s="25"/>
     </row>
-    <row r="64" spans="1:22" s="16" customFormat="1" ht="24">
+    <row r="64" spans="1:22" s="16" customFormat="1" ht="25">
       <c r="A64" s="31" t="s">
         <v>189</v>
       </c>
@@ -3488,6 +3853,9 @@
       </c>
       <c r="D64" s="21">
         <v>3</v>
+      </c>
+      <c r="E64" s="40" t="s">
+        <v>242</v>
       </c>
       <c r="F64" s="27" t="s">
         <v>209</v>
@@ -3511,7 +3879,7 @@
       <c r="U64" s="25"/>
       <c r="V64" s="25"/>
     </row>
-    <row r="65" spans="1:22" s="16" customFormat="1" ht="24">
+    <row r="65" spans="1:22" s="16" customFormat="1" ht="25">
       <c r="A65" s="31" t="s">
         <v>190</v>
       </c>
@@ -3523,6 +3891,9 @@
       </c>
       <c r="D65" s="21">
         <v>4</v>
+      </c>
+      <c r="E65" s="40" t="s">
+        <v>287</v>
       </c>
       <c r="F65" s="27" t="s">
         <v>222</v>
@@ -3546,7 +3917,7 @@
       <c r="U65" s="25"/>
       <c r="V65" s="25"/>
     </row>
-    <row r="66" spans="1:22" s="16" customFormat="1" ht="24">
+    <row r="66" spans="1:22" s="16" customFormat="1" ht="25">
       <c r="A66" s="31" t="s">
         <v>191</v>
       </c>
@@ -3558,6 +3929,9 @@
       </c>
       <c r="D66" s="21">
         <v>5</v>
+      </c>
+      <c r="E66" s="40" t="s">
+        <v>288</v>
       </c>
       <c r="F66" s="27" t="s">
         <v>213</v>
@@ -3581,7 +3955,7 @@
       <c r="U66" s="25"/>
       <c r="V66" s="25"/>
     </row>
-    <row r="67" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="67" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A67" s="31" t="s">
         <v>192</v>
       </c>
@@ -3593,6 +3967,9 @@
       </c>
       <c r="D67" s="21">
         <v>6</v>
+      </c>
+      <c r="E67" s="40" t="s">
+        <v>289</v>
       </c>
       <c r="F67" s="27" t="s">
         <v>223</v>
@@ -3616,7 +3993,7 @@
       <c r="U67" s="25"/>
       <c r="V67" s="25"/>
     </row>
-    <row r="68" spans="1:22" s="16" customFormat="1" ht="48">
+    <row r="68" spans="1:22" s="16" customFormat="1" ht="49">
       <c r="A68" s="31" t="s">
         <v>193</v>
       </c>
@@ -3628,6 +4005,9 @@
       </c>
       <c r="D68" s="21">
         <v>7</v>
+      </c>
+      <c r="E68" s="40" t="s">
+        <v>290</v>
       </c>
       <c r="F68" s="27" t="s">
         <v>224</v>
@@ -3651,7 +4031,7 @@
       <c r="U68" s="25"/>
       <c r="V68" s="25"/>
     </row>
-    <row r="69" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="69" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A69" s="31" t="s">
         <v>194</v>
       </c>
@@ -3663,6 +4043,9 @@
       </c>
       <c r="D69" s="21">
         <v>8</v>
+      </c>
+      <c r="E69" s="40" t="s">
+        <v>291</v>
       </c>
       <c r="F69" s="22"/>
       <c r="G69" s="26" t="s">
@@ -3684,7 +4067,7 @@
       <c r="U69" s="25"/>
       <c r="V69" s="25"/>
     </row>
-    <row r="70" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="70" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A70" s="31" t="s">
         <v>195</v>
       </c>
@@ -3696,6 +4079,9 @@
       </c>
       <c r="D70" s="21">
         <v>9</v>
+      </c>
+      <c r="E70" s="40" t="s">
+        <v>292</v>
       </c>
       <c r="F70" s="27" t="s">
         <v>214</v>
@@ -3719,7 +4105,7 @@
       <c r="U70" s="25"/>
       <c r="V70" s="25"/>
     </row>
-    <row r="71" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="71" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A71" s="31" t="s">
         <v>196</v>
       </c>
@@ -3731,6 +4117,9 @@
       </c>
       <c r="D71" s="21">
         <v>10</v>
+      </c>
+      <c r="E71" s="40" t="s">
+        <v>293</v>
       </c>
       <c r="F71" s="22"/>
       <c r="G71" s="26" t="s">
@@ -3744,7 +4133,7 @@
       <c r="U71" s="25"/>
       <c r="V71" s="25"/>
     </row>
-    <row r="72" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="72" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A72" s="31" t="s">
         <v>197</v>
       </c>
@@ -3756,6 +4145,9 @@
       </c>
       <c r="D72" s="21">
         <v>11</v>
+      </c>
+      <c r="E72" s="40" t="s">
+        <v>294</v>
       </c>
       <c r="F72" s="22"/>
       <c r="G72" s="26" t="s">
@@ -3769,7 +4161,7 @@
       <c r="U72" s="25"/>
       <c r="V72" s="25"/>
     </row>
-    <row r="73" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="73" spans="1:22" s="16" customFormat="1" ht="28">
       <c r="A73" s="31" t="s">
         <v>198</v>
       </c>
@@ -3778,6 +4170,9 @@
       </c>
       <c r="C73" s="21">
         <v>3</v>
+      </c>
+      <c r="E73" s="40" t="s">
+        <v>295</v>
       </c>
       <c r="F73" s="22"/>
       <c r="G73" s="26" t="s">
@@ -3791,7 +4186,7 @@
       <c r="U73" s="25"/>
       <c r="V73" s="25"/>
     </row>
-    <row r="74" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="74" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A74" s="31" t="s">
         <v>199</v>
       </c>
@@ -3800,6 +4195,9 @@
       </c>
       <c r="C74" s="21">
         <v>4</v>
+      </c>
+      <c r="E74" s="40" t="s">
+        <v>21</v>
       </c>
       <c r="F74" s="22"/>
       <c r="G74" s="26" t="s">
@@ -3813,7 +4211,7 @@
       <c r="U74" s="25"/>
       <c r="V74" s="25"/>
     </row>
-    <row r="75" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="75" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A75" s="31" t="s">
         <v>200</v>
       </c>
@@ -3825,6 +4223,9 @@
       </c>
       <c r="D75" s="21">
         <v>0</v>
+      </c>
+      <c r="E75" s="40" t="s">
+        <v>296</v>
       </c>
       <c r="F75" s="22"/>
       <c r="G75" s="26" t="s">
@@ -3846,7 +4247,7 @@
       <c r="U75" s="25"/>
       <c r="V75" s="25"/>
     </row>
-    <row r="76" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="76" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A76" s="31" t="s">
         <v>201</v>
       </c>
@@ -3858,6 +4259,9 @@
       </c>
       <c r="D76" s="21">
         <v>1</v>
+      </c>
+      <c r="E76" s="40" t="s">
+        <v>297</v>
       </c>
       <c r="F76" s="27" t="s">
         <v>215</v>
@@ -3881,7 +4285,7 @@
       <c r="U76" s="25"/>
       <c r="V76" s="25"/>
     </row>
-    <row r="77" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="77" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A77" s="31" t="s">
         <v>202</v>
       </c>
@@ -3893,6 +4297,9 @@
       </c>
       <c r="D77" s="21">
         <v>2</v>
+      </c>
+      <c r="E77" s="40" t="s">
+        <v>298</v>
       </c>
       <c r="F77" s="27" t="s">
         <v>225</v>
@@ -3916,7 +4323,7 @@
       <c r="U77" s="25"/>
       <c r="V77" s="25"/>
     </row>
-    <row r="78" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="78" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A78" s="31" t="s">
         <v>203</v>
       </c>
@@ -3928,6 +4335,9 @@
       </c>
       <c r="D78" s="21">
         <v>3</v>
+      </c>
+      <c r="E78" s="40" t="s">
+        <v>299</v>
       </c>
       <c r="F78" s="22"/>
       <c r="G78" s="26" t="s">
@@ -3949,7 +4359,7 @@
       <c r="U78" s="25"/>
       <c r="V78" s="25"/>
     </row>
-    <row r="79" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="79" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A79" s="31" t="s">
         <v>204</v>
       </c>
@@ -3961,6 +4371,9 @@
       </c>
       <c r="D79" s="21">
         <v>4</v>
+      </c>
+      <c r="E79" s="40" t="s">
+        <v>300</v>
       </c>
       <c r="F79" s="27" t="s">
         <v>216</v>
@@ -3984,7 +4397,7 @@
       <c r="U79" s="25"/>
       <c r="V79" s="25"/>
     </row>
-    <row r="80" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="80" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A80" s="31" t="s">
         <v>205</v>
       </c>
@@ -3993,6 +4406,9 @@
       </c>
       <c r="C80" s="21">
         <v>5</v>
+      </c>
+      <c r="E80" s="40" t="s">
+        <v>301</v>
       </c>
       <c r="F80" s="22"/>
       <c r="G80" s="26" t="s">
@@ -4006,7 +4422,7 @@
       <c r="U80" s="25"/>
       <c r="V80" s="25"/>
     </row>
-    <row r="81" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="81" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A81" s="31" t="s">
         <v>206</v>
       </c>
@@ -4018,6 +4434,9 @@
       </c>
       <c r="D81" s="21">
         <v>0</v>
+      </c>
+      <c r="E81" s="40" t="s">
+        <v>302</v>
       </c>
       <c r="F81" s="22"/>
       <c r="G81" s="26" t="s">
@@ -4039,7 +4458,7 @@
       <c r="U81" s="25"/>
       <c r="V81" s="25"/>
     </row>
-    <row r="82" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="82" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A82" s="31" t="s">
         <v>207</v>
       </c>
@@ -4051,6 +4470,9 @@
       </c>
       <c r="D82" s="21">
         <v>1</v>
+      </c>
+      <c r="E82" s="40" t="s">
+        <v>303</v>
       </c>
       <c r="F82" s="22"/>
       <c r="G82" s="26" t="s">
@@ -4064,7 +4486,7 @@
       <c r="U82" s="25"/>
       <c r="V82" s="25"/>
     </row>
-    <row r="83" spans="1:22" s="16" customFormat="1" ht="12">
+    <row r="83" spans="1:22" s="16" customFormat="1" ht="14">
       <c r="A83" s="31" t="s">
         <v>208</v>
       </c>
@@ -4076,6 +4498,9 @@
       </c>
       <c r="D83" s="21">
         <v>2</v>
+      </c>
+      <c r="E83" s="40" t="s">
+        <v>304</v>
       </c>
       <c r="F83" s="22"/>
       <c r="G83" s="26" t="s">
@@ -4088,6 +4513,174 @@
       <c r="T83" s="25"/>
       <c r="U83" s="25"/>
       <c r="V83" s="25"/>
+    </row>
+    <row r="84" spans="1:22" ht="14">
+      <c r="E84" s="40"/>
+    </row>
+    <row r="85" spans="1:22" ht="14">
+      <c r="E85" s="40"/>
+    </row>
+    <row r="86" spans="1:22" ht="14">
+      <c r="E86" s="40"/>
+    </row>
+    <row r="87" spans="1:22" ht="14">
+      <c r="E87" s="40"/>
+    </row>
+    <row r="88" spans="1:22" ht="14">
+      <c r="E88" s="40"/>
+    </row>
+    <row r="89" spans="1:22" ht="14">
+      <c r="E89" s="40"/>
+    </row>
+    <row r="90" spans="1:22" ht="14">
+      <c r="E90" s="40"/>
+    </row>
+    <row r="91" spans="1:22" ht="14">
+      <c r="E91" s="40"/>
+    </row>
+    <row r="92" spans="1:22" ht="14">
+      <c r="E92" s="40"/>
+    </row>
+    <row r="93" spans="1:22" ht="14">
+      <c r="E93" s="40"/>
+    </row>
+    <row r="94" spans="1:22" ht="14">
+      <c r="E94" s="40"/>
+    </row>
+    <row r="95" spans="1:22" ht="14">
+      <c r="E95" s="40"/>
+    </row>
+    <row r="96" spans="1:22" ht="14">
+      <c r="E96" s="40"/>
+    </row>
+    <row r="97" spans="5:5" ht="14">
+      <c r="E97" s="40"/>
+    </row>
+    <row r="98" spans="5:5" ht="14">
+      <c r="E98" s="40"/>
+    </row>
+    <row r="99" spans="5:5" ht="14">
+      <c r="E99" s="40"/>
+    </row>
+    <row r="100" spans="5:5" ht="14">
+      <c r="E100" s="40"/>
+    </row>
+    <row r="101" spans="5:5" ht="14">
+      <c r="E101" s="40"/>
+    </row>
+    <row r="102" spans="5:5" ht="14">
+      <c r="E102" s="40"/>
+    </row>
+    <row r="103" spans="5:5" ht="14">
+      <c r="E103" s="40"/>
+    </row>
+    <row r="104" spans="5:5" ht="14">
+      <c r="E104" s="40"/>
+    </row>
+    <row r="105" spans="5:5" ht="14">
+      <c r="E105" s="40"/>
+    </row>
+    <row r="106" spans="5:5" ht="14">
+      <c r="E106" s="40"/>
+    </row>
+    <row r="107" spans="5:5" ht="14">
+      <c r="E107" s="40"/>
+    </row>
+    <row r="108" spans="5:5" ht="14">
+      <c r="E108" s="40"/>
+    </row>
+    <row r="109" spans="5:5" ht="14">
+      <c r="E109" s="40"/>
+    </row>
+    <row r="110" spans="5:5" ht="14">
+      <c r="E110" s="40"/>
+    </row>
+    <row r="111" spans="5:5" ht="14">
+      <c r="E111" s="40"/>
+    </row>
+    <row r="112" spans="5:5" ht="14">
+      <c r="E112" s="40"/>
+    </row>
+    <row r="113" spans="5:5" ht="14">
+      <c r="E113" s="40"/>
+    </row>
+    <row r="114" spans="5:5" ht="14">
+      <c r="E114" s="40"/>
+    </row>
+    <row r="115" spans="5:5" ht="14">
+      <c r="E115" s="40"/>
+    </row>
+    <row r="116" spans="5:5" ht="14">
+      <c r="E116" s="40"/>
+    </row>
+    <row r="117" spans="5:5" ht="14">
+      <c r="E117" s="40"/>
+    </row>
+    <row r="118" spans="5:5" ht="14">
+      <c r="E118" s="40"/>
+    </row>
+    <row r="119" spans="5:5" ht="14">
+      <c r="E119" s="40"/>
+    </row>
+    <row r="120" spans="5:5" ht="14">
+      <c r="E120" s="40"/>
+    </row>
+    <row r="121" spans="5:5" ht="14">
+      <c r="E121" s="40"/>
+    </row>
+    <row r="122" spans="5:5" ht="14">
+      <c r="E122" s="40"/>
+    </row>
+    <row r="123" spans="5:5" ht="14">
+      <c r="E123" s="40"/>
+    </row>
+    <row r="124" spans="5:5" ht="14">
+      <c r="E124" s="40"/>
+    </row>
+    <row r="125" spans="5:5" ht="14">
+      <c r="E125" s="40"/>
+    </row>
+    <row r="126" spans="5:5" ht="14">
+      <c r="E126" s="40"/>
+    </row>
+    <row r="127" spans="5:5" ht="14">
+      <c r="E127" s="40"/>
+    </row>
+    <row r="128" spans="5:5" ht="14">
+      <c r="E128" s="40"/>
+    </row>
+    <row r="129" spans="5:5" ht="14">
+      <c r="E129" s="40"/>
+    </row>
+    <row r="130" spans="5:5" ht="14">
+      <c r="E130" s="40"/>
+    </row>
+    <row r="131" spans="5:5" ht="14">
+      <c r="E131" s="40"/>
+    </row>
+    <row r="132" spans="5:5" ht="14">
+      <c r="E132" s="40"/>
+    </row>
+    <row r="133" spans="5:5" ht="14">
+      <c r="E133" s="40"/>
+    </row>
+    <row r="134" spans="5:5" ht="14">
+      <c r="E134" s="40"/>
+    </row>
+    <row r="135" spans="5:5" ht="14">
+      <c r="E135" s="40"/>
+    </row>
+    <row r="136" spans="5:5" ht="14">
+      <c r="E136" s="40"/>
+    </row>
+    <row r="137" spans="5:5" ht="14">
+      <c r="E137" s="40"/>
+    </row>
+    <row r="138" spans="5:5" ht="14">
+      <c r="E138" s="40"/>
+    </row>
+    <row r="139" spans="5:5" ht="14">
+      <c r="E139" s="40"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>

<commit_message>
Remove duplicate entry in repo-minimal template.
</commit_message>
<xml_diff>
--- a/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/ordnungssystem.xlsx
+++ b/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/ordnungssystem.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="304">
   <si>
     <t>reference_number</t>
   </si>
@@ -2063,13 +2063,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blatt1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:U545"/>
+  <dimension ref="A1:U544"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2992,13 +2992,13 @@
     </row>
     <row r="31" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A31" s="19" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="27" t="s">
@@ -3015,17 +3015,26 @@
     </row>
     <row r="32" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A32" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="27" t="s">
         <v>26</v>
+      </c>
+      <c r="H32" s="27">
+        <v>10</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="M32" s="28"/>
       <c r="N32" s="25"/>
@@ -3038,26 +3047,17 @@
     </row>
     <row r="33" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="27" t="s">
         <v>26</v>
-      </c>
-      <c r="H33" s="27">
-        <v>10</v>
-      </c>
-      <c r="I33" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="J33" s="27" t="s">
-        <v>32</v>
       </c>
       <c r="M33" s="28"/>
       <c r="N33" s="25"/>
@@ -3070,13 +3070,13 @@
     </row>
     <row r="34" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="27" t="s">
@@ -3093,13 +3093,13 @@
     </row>
     <row r="35" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="27" t="s">
@@ -3116,13 +3116,13 @@
     </row>
     <row r="36" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="27" t="s">
@@ -3139,15 +3139,17 @@
     </row>
     <row r="37" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="D37" s="21"/>
+        <v>240</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>284</v>
+      </c>
       <c r="E37" s="27" t="s">
         <v>26</v>
       </c>
@@ -3162,17 +3164,15 @@
     </row>
     <row r="38" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>284</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="D38" s="21"/>
       <c r="E38" s="27" t="s">
         <v>26</v>
       </c>
@@ -3187,13 +3187,13 @@
     </row>
     <row r="39" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="27" t="s">
@@ -3210,13 +3210,13 @@
     </row>
     <row r="40" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="27" t="s">
@@ -3233,13 +3233,13 @@
     </row>
     <row r="41" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="27" t="s">
@@ -3256,13 +3256,13 @@
     </row>
     <row r="42" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="27" t="s">
@@ -3279,13 +3279,13 @@
     </row>
     <row r="43" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="27" t="s">
@@ -3302,13 +3302,13 @@
     </row>
     <row r="44" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="27" t="s">
@@ -3325,13 +3325,13 @@
     </row>
     <row r="45" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D45" s="21"/>
       <c r="E45" s="27" t="s">
@@ -3348,17 +3348,26 @@
     </row>
     <row r="46" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="D46" s="21"/>
       <c r="E46" s="27" t="s">
         <v>26</v>
+      </c>
+      <c r="H46" s="27">
+        <v>10</v>
+      </c>
+      <c r="I46" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="J46" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="M46" s="28"/>
       <c r="N46" s="25"/>
@@ -3371,26 +3380,17 @@
     </row>
     <row r="47" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A47" s="19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="D47" s="21"/>
       <c r="E47" s="27" t="s">
         <v>26</v>
-      </c>
-      <c r="H47" s="27">
-        <v>10</v>
-      </c>
-      <c r="I47" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="J47" s="27" t="s">
-        <v>32</v>
       </c>
       <c r="M47" s="28"/>
       <c r="N47" s="25"/>
@@ -3403,17 +3403,26 @@
     </row>
     <row r="48" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A48" s="19" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="27" t="s">
         <v>26</v>
+      </c>
+      <c r="H48" s="27">
+        <v>50</v>
+      </c>
+      <c r="I48" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="J48" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="M48" s="28"/>
       <c r="N48" s="25"/>
@@ -3426,23 +3435,23 @@
     </row>
     <row r="49" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>250</v>
+        <v>152</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>251</v>
       </c>
       <c r="D49" s="21"/>
       <c r="E49" s="27" t="s">
         <v>26</v>
       </c>
       <c r="H49" s="27">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="I49" s="27" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J49" s="27" t="s">
         <v>32</v>
@@ -3458,23 +3467,25 @@
     </row>
     <row r="50" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="D50" s="21"/>
+        <v>252</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>285</v>
+      </c>
       <c r="E50" s="27" t="s">
         <v>26</v>
       </c>
       <c r="H50" s="27">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="I50" s="27" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J50" s="27" t="s">
         <v>32</v>
@@ -3490,17 +3501,15 @@
     </row>
     <row r="51" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A51" s="19" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="D51" s="21" t="s">
-        <v>285</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="D51" s="21"/>
       <c r="E51" s="27" t="s">
         <v>26</v>
       </c>
@@ -3524,26 +3533,17 @@
     </row>
     <row r="52" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A52" s="19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D52" s="21"/>
       <c r="E52" s="27" t="s">
         <v>26</v>
-      </c>
-      <c r="H52" s="27">
-        <v>50</v>
-      </c>
-      <c r="I52" s="27" t="s">
-        <v>299</v>
-      </c>
-      <c r="J52" s="27" t="s">
-        <v>32</v>
       </c>
       <c r="M52" s="28"/>
       <c r="N52" s="25"/>
@@ -3556,13 +3556,13 @@
     </row>
     <row r="53" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A53" s="19" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C53" s="30" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="27" t="s">
@@ -3579,17 +3579,26 @@
     </row>
     <row r="54" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A54" s="19" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="27" t="s">
         <v>26</v>
+      </c>
+      <c r="H54" s="27">
+        <v>10</v>
+      </c>
+      <c r="I54" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="J54" s="27" t="s">
+        <v>33</v>
       </c>
       <c r="M54" s="28"/>
       <c r="N54" s="25"/>
@@ -3602,15 +3611,17 @@
     </row>
     <row r="55" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A55" s="19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C55" s="30" t="s">
-        <v>256</v>
-      </c>
-      <c r="D55" s="21"/>
+        <v>257</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>286</v>
+      </c>
       <c r="E55" s="27" t="s">
         <v>26</v>
       </c>
@@ -3618,10 +3629,10 @@
         <v>10</v>
       </c>
       <c r="I55" s="27" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J55" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M55" s="28"/>
       <c r="N55" s="25"/>
@@ -3634,17 +3645,15 @@
     </row>
     <row r="56" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A56" s="19" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>257</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>286</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="D56" s="21"/>
       <c r="E56" s="27" t="s">
         <v>26</v>
       </c>
@@ -3652,10 +3661,10 @@
         <v>10</v>
       </c>
       <c r="I56" s="27" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J56" s="27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M56" s="28"/>
       <c r="N56" s="25"/>
@@ -3668,26 +3677,26 @@
     </row>
     <row r="57" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A57" s="19" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C57" s="30" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="27" t="s">
         <v>26</v>
       </c>
       <c r="H57" s="27">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I57" s="27" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="J57" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M57" s="28"/>
       <c r="N57" s="25"/>
@@ -3700,26 +3709,17 @@
     </row>
     <row r="58" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A58" s="19" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="27" t="s">
         <v>26</v>
-      </c>
-      <c r="H58" s="27">
-        <v>30</v>
-      </c>
-      <c r="I58" s="27" t="s">
-        <v>301</v>
-      </c>
-      <c r="J58" s="27" t="s">
-        <v>34</v>
       </c>
       <c r="M58" s="28"/>
       <c r="N58" s="25"/>
@@ -3732,13 +3732,13 @@
     </row>
     <row r="59" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A59" s="19" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C59" s="30" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="27" t="s">
@@ -3755,17 +3755,28 @@
     </row>
     <row r="60" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A60" s="19" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>172</v>
+        <v>89</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>261</v>
-      </c>
-      <c r="D60" s="21"/>
+        <v>223</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>287</v>
+      </c>
       <c r="E60" s="27" t="s">
         <v>26</v>
+      </c>
+      <c r="H60" s="27">
+        <v>10</v>
+      </c>
+      <c r="I60" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="J60" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="M60" s="28"/>
       <c r="N60" s="25"/>
@@ -3778,17 +3789,15 @@
     </row>
     <row r="61" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A61" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>89</v>
+        <v>175</v>
       </c>
       <c r="C61" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="D61" s="21" t="s">
-        <v>287</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="D61" s="21"/>
       <c r="E61" s="27" t="s">
         <v>26</v>
       </c>
@@ -3799,7 +3808,7 @@
         <v>297</v>
       </c>
       <c r="J61" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M61" s="28"/>
       <c r="N61" s="25"/>
@@ -3812,26 +3821,17 @@
     </row>
     <row r="62" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A62" s="19" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C62" s="30" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="27" t="s">
         <v>26</v>
-      </c>
-      <c r="H62" s="27">
-        <v>10</v>
-      </c>
-      <c r="I62" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="J62" s="27" t="s">
-        <v>34</v>
       </c>
       <c r="M62" s="28"/>
       <c r="N62" s="25"/>
@@ -3844,17 +3844,28 @@
     </row>
     <row r="63" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A63" s="19" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C63" s="30" t="s">
-        <v>263</v>
-      </c>
-      <c r="D63" s="21"/>
+        <v>264</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>288</v>
+      </c>
       <c r="E63" s="27" t="s">
         <v>26</v>
+      </c>
+      <c r="H63" s="27">
+        <v>10</v>
+      </c>
+      <c r="I63" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="J63" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="M63" s="28"/>
       <c r="N63" s="25"/>
@@ -3867,16 +3878,16 @@
     </row>
     <row r="64" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A64" s="19" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C64" s="30" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E64" s="27" t="s">
         <v>26</v>
@@ -3885,7 +3896,7 @@
         <v>10</v>
       </c>
       <c r="I64" s="27" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="J64" s="27" t="s">
         <v>34</v>
@@ -3901,16 +3912,16 @@
     </row>
     <row r="65" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A65" s="19" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E65" s="27" t="s">
         <v>26</v>
@@ -3919,7 +3930,7 @@
         <v>10</v>
       </c>
       <c r="I65" s="27" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="J65" s="27" t="s">
         <v>34</v>
@@ -3935,16 +3946,16 @@
     </row>
     <row r="66" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A66" s="19" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C66" s="30" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E66" s="27" t="s">
         <v>26</v>
@@ -3969,16 +3980,16 @@
     </row>
     <row r="67" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A67" s="19" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C67" s="30" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E67" s="27" t="s">
         <v>26</v>
@@ -4003,17 +4014,15 @@
     </row>
     <row r="68" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A68" s="19" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C68" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="D68" s="21" t="s">
-        <v>292</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="D68" s="21"/>
       <c r="E68" s="27" t="s">
         <v>26</v>
       </c>
@@ -4024,7 +4033,7 @@
         <v>297</v>
       </c>
       <c r="J68" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M68" s="28"/>
       <c r="N68" s="25"/>
@@ -4037,15 +4046,17 @@
     </row>
     <row r="69" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A69" s="19" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C69" s="30" t="s">
-        <v>269</v>
-      </c>
-      <c r="D69" s="21"/>
+        <v>241</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>293</v>
+      </c>
       <c r="E69" s="27" t="s">
         <v>26</v>
       </c>
@@ -4069,28 +4080,17 @@
     </row>
     <row r="70" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A70" s="19" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C70" s="30" t="s">
-        <v>241</v>
-      </c>
-      <c r="D70" s="21" t="s">
-        <v>293</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="D70" s="21"/>
       <c r="E70" s="27" t="s">
         <v>26</v>
-      </c>
-      <c r="H70" s="27">
-        <v>10</v>
-      </c>
-      <c r="I70" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="J70" s="27" t="s">
-        <v>33</v>
       </c>
       <c r="M70" s="28"/>
       <c r="N70" s="25"/>
@@ -4103,13 +4103,13 @@
     </row>
     <row r="71" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A71" s="19" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C71" s="30" t="s">
-        <v>193</v>
+        <v>270</v>
       </c>
       <c r="D71" s="21"/>
       <c r="E71" s="27" t="s">
@@ -4126,13 +4126,13 @@
     </row>
     <row r="72" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A72" s="19" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C72" s="30" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="27" t="s">
@@ -4149,13 +4149,13 @@
     </row>
     <row r="73" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A73" s="19" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C73" s="30" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D73" s="21"/>
       <c r="E73" s="27" t="s">
@@ -4172,17 +4172,26 @@
     </row>
     <row r="74" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A74" s="19" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>199</v>
+        <v>89</v>
       </c>
       <c r="C74" s="30" t="s">
-        <v>272</v>
+        <v>223</v>
       </c>
       <c r="D74" s="21"/>
       <c r="E74" s="27" t="s">
         <v>26</v>
+      </c>
+      <c r="H74" s="27">
+        <v>10</v>
+      </c>
+      <c r="I74" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="J74" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="M74" s="28"/>
       <c r="N74" s="25"/>
@@ -4195,15 +4204,17 @@
     </row>
     <row r="75" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A75" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>89</v>
+        <v>202</v>
       </c>
       <c r="C75" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="D75" s="21"/>
+        <v>273</v>
+      </c>
+      <c r="D75" s="21" t="s">
+        <v>294</v>
+      </c>
       <c r="E75" s="27" t="s">
         <v>26</v>
       </c>
@@ -4214,7 +4225,7 @@
         <v>297</v>
       </c>
       <c r="J75" s="27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M75" s="28"/>
       <c r="N75" s="25"/>
@@ -4227,16 +4238,16 @@
     </row>
     <row r="76" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A76" s="19" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C76" s="30" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E76" s="27" t="s">
         <v>26</v>
@@ -4261,17 +4272,15 @@
     </row>
     <row r="77" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A77" s="19" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C77" s="30" t="s">
-        <v>274</v>
-      </c>
-      <c r="D77" s="21" t="s">
-        <v>295</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="D77" s="21"/>
       <c r="E77" s="27" t="s">
         <v>26</v>
       </c>
@@ -4295,15 +4304,17 @@
     </row>
     <row r="78" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A78" s="19" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C78" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="D78" s="21"/>
+        <v>276</v>
+      </c>
+      <c r="D78" s="21" t="s">
+        <v>296</v>
+      </c>
       <c r="E78" s="27" t="s">
         <v>26</v>
       </c>
@@ -4327,28 +4338,20 @@
     </row>
     <row r="79" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A79" s="19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C79" s="30" t="s">
-        <v>276</v>
-      </c>
-      <c r="D79" s="21" t="s">
-        <v>296</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="D79" s="21"/>
       <c r="E79" s="27" t="s">
         <v>26</v>
       </c>
       <c r="H79" s="27">
-        <v>10</v>
-      </c>
-      <c r="I79" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="J79" s="27" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="M79" s="28"/>
       <c r="N79" s="25"/>
@@ -4361,17 +4364,26 @@
     </row>
     <row r="80" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A80" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>210</v>
+        <v>89</v>
       </c>
       <c r="C80" s="30" t="s">
-        <v>277</v>
+        <v>223</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="27" t="s">
         <v>26</v>
+      </c>
+      <c r="H80" s="27">
+        <v>10</v>
+      </c>
+      <c r="I80" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="J80" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="M80" s="28"/>
       <c r="N80" s="25"/>
@@ -4384,26 +4396,17 @@
     </row>
     <row r="81" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A81" s="19" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>89</v>
+        <v>213</v>
       </c>
       <c r="C81" s="30" t="s">
-        <v>223</v>
+        <v>278</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="27" t="s">
         <v>26</v>
-      </c>
-      <c r="H81" s="27">
-        <v>10</v>
-      </c>
-      <c r="I81" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="J81" s="27" t="s">
-        <v>32</v>
       </c>
       <c r="M81" s="28"/>
       <c r="N81" s="25"/>
@@ -4416,13 +4419,13 @@
     </row>
     <row r="82" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
       <c r="A82" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C82" s="30" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="27" t="s">
@@ -4437,28 +4440,27 @@
       <c r="S82" s="29"/>
       <c r="T82" s="29"/>
     </row>
-    <row r="83" spans="1:20" s="27" customFormat="1" ht="13" customHeight="1">
-      <c r="A83" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="C83" s="30" t="s">
-        <v>279</v>
-      </c>
-      <c r="D83" s="21"/>
-      <c r="E83" s="27" t="s">
-        <v>26</v>
-      </c>
+    <row r="83" spans="1:20" ht="13" customHeight="1">
+      <c r="A83" s="31"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="32"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="27"/>
+      <c r="I83" s="27"/>
+      <c r="J83" s="27"/>
+      <c r="K83" s="27"/>
+      <c r="L83" s="27"/>
       <c r="M83" s="28"/>
       <c r="N83" s="25"/>
-      <c r="O83" s="29"/>
-      <c r="P83" s="29"/>
-      <c r="Q83" s="29"/>
-      <c r="R83" s="29"/>
-      <c r="S83" s="29"/>
-      <c r="T83" s="29"/>
+      <c r="O83" s="33"/>
+      <c r="P83" s="34"/>
+      <c r="Q83" s="34"/>
+      <c r="R83" s="34"/>
+      <c r="S83" s="34"/>
+      <c r="T83" s="34"/>
     </row>
     <row r="84" spans="1:20" ht="13" customHeight="1">
       <c r="A84" s="31"/>
@@ -4475,12 +4477,12 @@
       <c r="L84" s="27"/>
       <c r="M84" s="28"/>
       <c r="N84" s="25"/>
-      <c r="O84" s="33"/>
-      <c r="P84" s="34"/>
-      <c r="Q84" s="34"/>
-      <c r="R84" s="34"/>
-      <c r="S84" s="34"/>
-      <c r="T84" s="34"/>
+      <c r="O84" s="36"/>
+      <c r="P84" s="37"/>
+      <c r="Q84" s="37"/>
+      <c r="R84" s="37"/>
+      <c r="S84" s="37"/>
+      <c r="T84" s="37"/>
     </row>
     <row r="85" spans="1:20" ht="13" customHeight="1">
       <c r="A85" s="31"/>
@@ -4772,7 +4774,7 @@
       <c r="A98" s="31"/>
       <c r="B98" s="27"/>
       <c r="C98" s="30"/>
-      <c r="D98" s="32"/>
+      <c r="D98" s="38"/>
       <c r="E98" s="27"/>
       <c r="F98" s="27"/>
       <c r="G98" s="27"/>
@@ -4882,7 +4884,7 @@
       <c r="A103" s="31"/>
       <c r="B103" s="27"/>
       <c r="C103" s="30"/>
-      <c r="D103" s="38"/>
+      <c r="D103" s="32"/>
       <c r="E103" s="27"/>
       <c r="F103" s="27"/>
       <c r="G103" s="27"/>
@@ -4945,10 +4947,10 @@
       <c r="T105" s="37"/>
     </row>
     <row r="106" spans="1:20" ht="13" customHeight="1">
-      <c r="A106" s="31"/>
+      <c r="A106" s="39"/>
       <c r="B106" s="27"/>
       <c r="C106" s="30"/>
-      <c r="D106" s="32"/>
+      <c r="D106" s="40"/>
       <c r="E106" s="27"/>
       <c r="F106" s="27"/>
       <c r="G106" s="27"/>
@@ -4967,10 +4969,10 @@
       <c r="T106" s="37"/>
     </row>
     <row r="107" spans="1:20" ht="13" customHeight="1">
-      <c r="A107" s="39"/>
+      <c r="A107" s="31"/>
       <c r="B107" s="27"/>
       <c r="C107" s="30"/>
-      <c r="D107" s="40"/>
+      <c r="D107" s="41"/>
       <c r="E107" s="27"/>
       <c r="F107" s="27"/>
       <c r="G107" s="27"/>
@@ -4992,7 +4994,7 @@
       <c r="A108" s="31"/>
       <c r="B108" s="27"/>
       <c r="C108" s="30"/>
-      <c r="D108" s="41"/>
+      <c r="D108" s="32"/>
       <c r="E108" s="27"/>
       <c r="F108" s="27"/>
       <c r="G108" s="27"/>
@@ -5234,7 +5236,7 @@
       <c r="A119" s="31"/>
       <c r="B119" s="27"/>
       <c r="C119" s="30"/>
-      <c r="D119" s="32"/>
+      <c r="D119" s="40"/>
       <c r="E119" s="27"/>
       <c r="F119" s="27"/>
       <c r="G119" s="27"/>
@@ -5256,7 +5258,7 @@
       <c r="A120" s="31"/>
       <c r="B120" s="27"/>
       <c r="C120" s="30"/>
-      <c r="D120" s="40"/>
+      <c r="D120" s="32"/>
       <c r="E120" s="27"/>
       <c r="F120" s="27"/>
       <c r="G120" s="27"/>
@@ -5410,7 +5412,7 @@
       <c r="A127" s="31"/>
       <c r="B127" s="27"/>
       <c r="C127" s="30"/>
-      <c r="D127" s="32"/>
+      <c r="D127" s="38"/>
       <c r="E127" s="27"/>
       <c r="F127" s="27"/>
       <c r="G127" s="27"/>
@@ -5432,7 +5434,7 @@
       <c r="A128" s="31"/>
       <c r="B128" s="27"/>
       <c r="C128" s="30"/>
-      <c r="D128" s="38"/>
+      <c r="D128" s="32"/>
       <c r="E128" s="27"/>
       <c r="F128" s="27"/>
       <c r="G128" s="27"/>
@@ -5454,7 +5456,7 @@
       <c r="A129" s="31"/>
       <c r="B129" s="27"/>
       <c r="C129" s="30"/>
-      <c r="D129" s="32"/>
+      <c r="D129" s="42"/>
       <c r="E129" s="27"/>
       <c r="F129" s="27"/>
       <c r="G129" s="27"/>
@@ -5476,7 +5478,7 @@
       <c r="A130" s="31"/>
       <c r="B130" s="27"/>
       <c r="C130" s="30"/>
-      <c r="D130" s="42"/>
+      <c r="D130" s="43"/>
       <c r="E130" s="27"/>
       <c r="F130" s="27"/>
       <c r="G130" s="27"/>
@@ -5498,7 +5500,7 @@
       <c r="A131" s="31"/>
       <c r="B131" s="27"/>
       <c r="C131" s="30"/>
-      <c r="D131" s="43"/>
+      <c r="D131" s="44"/>
       <c r="E131" s="27"/>
       <c r="F131" s="27"/>
       <c r="G131" s="27"/>
@@ -5564,7 +5566,7 @@
       <c r="A134" s="31"/>
       <c r="B134" s="27"/>
       <c r="C134" s="30"/>
-      <c r="D134" s="44"/>
+      <c r="D134" s="32"/>
       <c r="E134" s="27"/>
       <c r="F134" s="27"/>
       <c r="G134" s="27"/>
@@ -5586,7 +5588,7 @@
       <c r="A135" s="31"/>
       <c r="B135" s="27"/>
       <c r="C135" s="30"/>
-      <c r="D135" s="32"/>
+      <c r="D135" s="45"/>
       <c r="E135" s="27"/>
       <c r="F135" s="27"/>
       <c r="G135" s="27"/>
@@ -5762,7 +5764,7 @@
       <c r="A143" s="31"/>
       <c r="B143" s="27"/>
       <c r="C143" s="30"/>
-      <c r="D143" s="45"/>
+      <c r="D143" s="32"/>
       <c r="E143" s="27"/>
       <c r="F143" s="27"/>
       <c r="G143" s="27"/>
@@ -5850,7 +5852,7 @@
       <c r="A147" s="31"/>
       <c r="B147" s="27"/>
       <c r="C147" s="30"/>
-      <c r="D147" s="32"/>
+      <c r="D147" s="40"/>
       <c r="E147" s="27"/>
       <c r="F147" s="27"/>
       <c r="G147" s="27"/>
@@ -5872,7 +5874,7 @@
       <c r="A148" s="31"/>
       <c r="B148" s="27"/>
       <c r="C148" s="30"/>
-      <c r="D148" s="40"/>
+      <c r="D148" s="32"/>
       <c r="E148" s="27"/>
       <c r="F148" s="27"/>
       <c r="G148" s="27"/>
@@ -5916,7 +5918,7 @@
       <c r="A150" s="31"/>
       <c r="B150" s="27"/>
       <c r="C150" s="30"/>
-      <c r="D150" s="32"/>
+      <c r="D150" s="46"/>
       <c r="E150" s="27"/>
       <c r="F150" s="27"/>
       <c r="G150" s="27"/>
@@ -5938,7 +5940,7 @@
       <c r="A151" s="31"/>
       <c r="B151" s="27"/>
       <c r="C151" s="30"/>
-      <c r="D151" s="46"/>
+      <c r="D151" s="47"/>
       <c r="E151" s="27"/>
       <c r="F151" s="27"/>
       <c r="G151" s="27"/>
@@ -5960,7 +5962,7 @@
       <c r="A152" s="31"/>
       <c r="B152" s="27"/>
       <c r="C152" s="30"/>
-      <c r="D152" s="47"/>
+      <c r="D152" s="32"/>
       <c r="E152" s="27"/>
       <c r="F152" s="27"/>
       <c r="G152" s="27"/>
@@ -6136,7 +6138,7 @@
       <c r="A160" s="31"/>
       <c r="B160" s="27"/>
       <c r="C160" s="30"/>
-      <c r="D160" s="32"/>
+      <c r="D160" s="40"/>
       <c r="E160" s="27"/>
       <c r="F160" s="27"/>
       <c r="G160" s="27"/>
@@ -6290,7 +6292,7 @@
       <c r="A167" s="31"/>
       <c r="B167" s="27"/>
       <c r="C167" s="30"/>
-      <c r="D167" s="40"/>
+      <c r="D167" s="32"/>
       <c r="E167" s="27"/>
       <c r="F167" s="27"/>
       <c r="G167" s="27"/>
@@ -6708,7 +6710,7 @@
       <c r="A186" s="31"/>
       <c r="B186" s="27"/>
       <c r="C186" s="30"/>
-      <c r="D186" s="32"/>
+      <c r="D186" s="40"/>
       <c r="E186" s="27"/>
       <c r="F186" s="27"/>
       <c r="G186" s="27"/>
@@ -6840,7 +6842,7 @@
       <c r="A192" s="31"/>
       <c r="B192" s="27"/>
       <c r="C192" s="30"/>
-      <c r="D192" s="40"/>
+      <c r="D192" s="32"/>
       <c r="E192" s="27"/>
       <c r="F192" s="27"/>
       <c r="G192" s="27"/>
@@ -7456,7 +7458,7 @@
       <c r="A220" s="31"/>
       <c r="B220" s="27"/>
       <c r="C220" s="30"/>
-      <c r="D220" s="32"/>
+      <c r="D220" s="40"/>
       <c r="E220" s="27"/>
       <c r="F220" s="27"/>
       <c r="G220" s="27"/>
@@ -7632,7 +7634,7 @@
       <c r="A228" s="31"/>
       <c r="B228" s="27"/>
       <c r="C228" s="30"/>
-      <c r="D228" s="40"/>
+      <c r="D228" s="32"/>
       <c r="E228" s="27"/>
       <c r="F228" s="27"/>
       <c r="G228" s="27"/>
@@ -8028,7 +8030,7 @@
       <c r="A246" s="31"/>
       <c r="B246" s="27"/>
       <c r="C246" s="30"/>
-      <c r="D246" s="32"/>
+      <c r="D246" s="40"/>
       <c r="E246" s="27"/>
       <c r="F246" s="27"/>
       <c r="G246" s="27"/>
@@ -8116,7 +8118,7 @@
       <c r="A250" s="31"/>
       <c r="B250" s="27"/>
       <c r="C250" s="30"/>
-      <c r="D250" s="40"/>
+      <c r="D250" s="32"/>
       <c r="E250" s="27"/>
       <c r="F250" s="27"/>
       <c r="G250" s="27"/>
@@ -8402,7 +8404,7 @@
       <c r="A263" s="31"/>
       <c r="B263" s="27"/>
       <c r="C263" s="30"/>
-      <c r="D263" s="32"/>
+      <c r="D263" s="40"/>
       <c r="E263" s="27"/>
       <c r="F263" s="27"/>
       <c r="G263" s="27"/>
@@ -8446,7 +8448,7 @@
       <c r="A265" s="31"/>
       <c r="B265" s="27"/>
       <c r="C265" s="30"/>
-      <c r="D265" s="40"/>
+      <c r="D265" s="32"/>
       <c r="E265" s="27"/>
       <c r="F265" s="27"/>
       <c r="G265" s="27"/>
@@ -8556,7 +8558,7 @@
       <c r="A270" s="31"/>
       <c r="B270" s="27"/>
       <c r="C270" s="30"/>
-      <c r="D270" s="32"/>
+      <c r="D270" s="40"/>
       <c r="E270" s="27"/>
       <c r="F270" s="27"/>
       <c r="G270" s="27"/>
@@ -8600,7 +8602,7 @@
       <c r="A272" s="31"/>
       <c r="B272" s="27"/>
       <c r="C272" s="30"/>
-      <c r="D272" s="40"/>
+      <c r="D272" s="32"/>
       <c r="E272" s="27"/>
       <c r="F272" s="27"/>
       <c r="G272" s="27"/>
@@ -8666,7 +8668,7 @@
       <c r="A275" s="31"/>
       <c r="B275" s="27"/>
       <c r="C275" s="30"/>
-      <c r="D275" s="32"/>
+      <c r="D275" s="40"/>
       <c r="E275" s="27"/>
       <c r="F275" s="27"/>
       <c r="G275" s="27"/>
@@ -8710,7 +8712,7 @@
       <c r="A277" s="31"/>
       <c r="B277" s="27"/>
       <c r="C277" s="30"/>
-      <c r="D277" s="40"/>
+      <c r="D277" s="32"/>
       <c r="E277" s="27"/>
       <c r="F277" s="27"/>
       <c r="G277" s="27"/>
@@ -9018,7 +9020,7 @@
       <c r="A291" s="31"/>
       <c r="B291" s="27"/>
       <c r="C291" s="30"/>
-      <c r="D291" s="32"/>
+      <c r="D291" s="40"/>
       <c r="E291" s="27"/>
       <c r="F291" s="27"/>
       <c r="G291" s="27"/>
@@ -9062,7 +9064,7 @@
       <c r="A293" s="31"/>
       <c r="B293" s="27"/>
       <c r="C293" s="30"/>
-      <c r="D293" s="40"/>
+      <c r="D293" s="32"/>
       <c r="E293" s="27"/>
       <c r="F293" s="27"/>
       <c r="G293" s="27"/>
@@ -9216,7 +9218,7 @@
       <c r="A300" s="31"/>
       <c r="B300" s="27"/>
       <c r="C300" s="30"/>
-      <c r="D300" s="32"/>
+      <c r="D300" s="40"/>
       <c r="E300" s="27"/>
       <c r="F300" s="27"/>
       <c r="G300" s="27"/>
@@ -9260,7 +9262,7 @@
       <c r="A302" s="31"/>
       <c r="B302" s="27"/>
       <c r="C302" s="30"/>
-      <c r="D302" s="40"/>
+      <c r="D302" s="32"/>
       <c r="E302" s="27"/>
       <c r="F302" s="27"/>
       <c r="G302" s="27"/>
@@ -9282,7 +9284,7 @@
       <c r="A303" s="31"/>
       <c r="B303" s="27"/>
       <c r="C303" s="30"/>
-      <c r="D303" s="32"/>
+      <c r="D303" s="46"/>
       <c r="E303" s="27"/>
       <c r="F303" s="27"/>
       <c r="G303" s="27"/>
@@ -9304,7 +9306,7 @@
       <c r="A304" s="31"/>
       <c r="B304" s="27"/>
       <c r="C304" s="30"/>
-      <c r="D304" s="46"/>
+      <c r="D304" s="47"/>
       <c r="E304" s="27"/>
       <c r="F304" s="27"/>
       <c r="G304" s="27"/>
@@ -9326,7 +9328,7 @@
       <c r="A305" s="31"/>
       <c r="B305" s="27"/>
       <c r="C305" s="30"/>
-      <c r="D305" s="47"/>
+      <c r="D305" s="32"/>
       <c r="E305" s="27"/>
       <c r="F305" s="27"/>
       <c r="G305" s="27"/>
@@ -9436,7 +9438,7 @@
       <c r="A310" s="31"/>
       <c r="B310" s="27"/>
       <c r="C310" s="30"/>
-      <c r="D310" s="32"/>
+      <c r="D310" s="40"/>
       <c r="E310" s="27"/>
       <c r="F310" s="27"/>
       <c r="G310" s="27"/>
@@ -9480,7 +9482,7 @@
       <c r="A312" s="31"/>
       <c r="B312" s="27"/>
       <c r="C312" s="30"/>
-      <c r="D312" s="40"/>
+      <c r="D312" s="32"/>
       <c r="E312" s="27"/>
       <c r="F312" s="27"/>
       <c r="G312" s="27"/>
@@ -9634,7 +9636,7 @@
       <c r="A319" s="31"/>
       <c r="B319" s="27"/>
       <c r="C319" s="30"/>
-      <c r="D319" s="32"/>
+      <c r="D319" s="40"/>
       <c r="E319" s="27"/>
       <c r="F319" s="27"/>
       <c r="G319" s="27"/>
@@ -9678,7 +9680,7 @@
       <c r="A321" s="31"/>
       <c r="B321" s="27"/>
       <c r="C321" s="30"/>
-      <c r="D321" s="40"/>
+      <c r="D321" s="32"/>
       <c r="E321" s="27"/>
       <c r="F321" s="27"/>
       <c r="G321" s="27"/>
@@ -9766,7 +9768,7 @@
       <c r="A325" s="31"/>
       <c r="B325" s="27"/>
       <c r="C325" s="30"/>
-      <c r="D325" s="32"/>
+      <c r="D325" s="40"/>
       <c r="E325" s="27"/>
       <c r="F325" s="27"/>
       <c r="G325" s="27"/>
@@ -9810,7 +9812,7 @@
       <c r="A327" s="31"/>
       <c r="B327" s="27"/>
       <c r="C327" s="30"/>
-      <c r="D327" s="40"/>
+      <c r="D327" s="32"/>
       <c r="E327" s="27"/>
       <c r="F327" s="27"/>
       <c r="G327" s="27"/>
@@ -9854,7 +9856,7 @@
       <c r="A329" s="31"/>
       <c r="B329" s="27"/>
       <c r="C329" s="30"/>
-      <c r="D329" s="32"/>
+      <c r="D329" s="40"/>
       <c r="E329" s="27"/>
       <c r="F329" s="27"/>
       <c r="G329" s="27"/>
@@ -9898,7 +9900,7 @@
       <c r="A331" s="31"/>
       <c r="B331" s="27"/>
       <c r="C331" s="30"/>
-      <c r="D331" s="40"/>
+      <c r="D331" s="32"/>
       <c r="E331" s="27"/>
       <c r="F331" s="27"/>
       <c r="G331" s="27"/>
@@ -9986,7 +9988,7 @@
       <c r="A335" s="31"/>
       <c r="B335" s="27"/>
       <c r="C335" s="30"/>
-      <c r="D335" s="32"/>
+      <c r="D335" s="40"/>
       <c r="E335" s="27"/>
       <c r="F335" s="27"/>
       <c r="G335" s="27"/>
@@ -10030,7 +10032,7 @@
       <c r="A337" s="31"/>
       <c r="B337" s="27"/>
       <c r="C337" s="30"/>
-      <c r="D337" s="40"/>
+      <c r="D337" s="32"/>
       <c r="E337" s="27"/>
       <c r="F337" s="27"/>
       <c r="G337" s="27"/>
@@ -10074,7 +10076,7 @@
       <c r="A339" s="31"/>
       <c r="B339" s="27"/>
       <c r="C339" s="30"/>
-      <c r="D339" s="32"/>
+      <c r="D339" s="40"/>
       <c r="E339" s="27"/>
       <c r="F339" s="27"/>
       <c r="G339" s="27"/>
@@ -10096,7 +10098,7 @@
       <c r="A340" s="31"/>
       <c r="B340" s="27"/>
       <c r="C340" s="30"/>
-      <c r="D340" s="40"/>
+      <c r="D340" s="32"/>
       <c r="E340" s="27"/>
       <c r="F340" s="27"/>
       <c r="G340" s="27"/>
@@ -10140,7 +10142,7 @@
       <c r="A342" s="31"/>
       <c r="B342" s="27"/>
       <c r="C342" s="30"/>
-      <c r="D342" s="32"/>
+      <c r="D342" s="40"/>
       <c r="E342" s="27"/>
       <c r="F342" s="27"/>
       <c r="G342" s="27"/>
@@ -10162,7 +10164,7 @@
       <c r="A343" s="31"/>
       <c r="B343" s="27"/>
       <c r="C343" s="30"/>
-      <c r="D343" s="40"/>
+      <c r="D343" s="32"/>
       <c r="E343" s="27"/>
       <c r="F343" s="27"/>
       <c r="G343" s="27"/>
@@ -10206,7 +10208,7 @@
       <c r="A345" s="31"/>
       <c r="B345" s="27"/>
       <c r="C345" s="30"/>
-      <c r="D345" s="32"/>
+      <c r="D345" s="40"/>
       <c r="E345" s="27"/>
       <c r="F345" s="27"/>
       <c r="G345" s="27"/>
@@ -10228,7 +10230,7 @@
       <c r="A346" s="31"/>
       <c r="B346" s="27"/>
       <c r="C346" s="30"/>
-      <c r="D346" s="40"/>
+      <c r="D346" s="32"/>
       <c r="E346" s="27"/>
       <c r="F346" s="27"/>
       <c r="G346" s="27"/>
@@ -10272,7 +10274,7 @@
       <c r="A348" s="31"/>
       <c r="B348" s="27"/>
       <c r="C348" s="30"/>
-      <c r="D348" s="32"/>
+      <c r="D348" s="40"/>
       <c r="E348" s="27"/>
       <c r="F348" s="27"/>
       <c r="G348" s="27"/>
@@ -10294,7 +10296,7 @@
       <c r="A349" s="31"/>
       <c r="B349" s="27"/>
       <c r="C349" s="30"/>
-      <c r="D349" s="40"/>
+      <c r="D349" s="32"/>
       <c r="E349" s="27"/>
       <c r="F349" s="27"/>
       <c r="G349" s="27"/>
@@ -10316,7 +10318,7 @@
       <c r="A350" s="31"/>
       <c r="B350" s="27"/>
       <c r="C350" s="30"/>
-      <c r="D350" s="32"/>
+      <c r="D350" s="42"/>
       <c r="E350" s="27"/>
       <c r="F350" s="27"/>
       <c r="G350" s="27"/>
@@ -11878,7 +11880,7 @@
       <c r="A421" s="31"/>
       <c r="B421" s="27"/>
       <c r="C421" s="30"/>
-      <c r="D421" s="42"/>
+      <c r="D421" s="27"/>
       <c r="E421" s="27"/>
       <c r="F421" s="27"/>
       <c r="G421" s="27"/>
@@ -11889,12 +11891,6 @@
       <c r="L421" s="27"/>
       <c r="M421" s="28"/>
       <c r="N421" s="25"/>
-      <c r="O421" s="36"/>
-      <c r="P421" s="37"/>
-      <c r="Q421" s="37"/>
-      <c r="R421" s="37"/>
-      <c r="S421" s="37"/>
-      <c r="T421" s="37"/>
     </row>
     <row r="422" spans="1:20" ht="13" customHeight="1">
       <c r="A422" s="31"/>
@@ -12108,7 +12104,7 @@
       <c r="A435" s="31"/>
       <c r="B435" s="27"/>
       <c r="C435" s="30"/>
-      <c r="D435" s="27"/>
+      <c r="D435" s="32"/>
       <c r="E435" s="27"/>
       <c r="F435" s="27"/>
       <c r="G435" s="27"/>
@@ -12119,12 +12115,18 @@
       <c r="L435" s="27"/>
       <c r="M435" s="28"/>
       <c r="N435" s="25"/>
+      <c r="O435" s="36"/>
+      <c r="P435" s="37"/>
+      <c r="Q435" s="37"/>
+      <c r="R435" s="37"/>
+      <c r="S435" s="37"/>
+      <c r="T435" s="37"/>
     </row>
     <row r="436" spans="1:20" ht="13" customHeight="1">
       <c r="A436" s="31"/>
       <c r="B436" s="27"/>
       <c r="C436" s="30"/>
-      <c r="D436" s="32"/>
+      <c r="D436" s="27"/>
       <c r="E436" s="27"/>
       <c r="F436" s="27"/>
       <c r="G436" s="27"/>
@@ -12135,12 +12137,6 @@
       <c r="L436" s="27"/>
       <c r="M436" s="28"/>
       <c r="N436" s="25"/>
-      <c r="O436" s="36"/>
-      <c r="P436" s="37"/>
-      <c r="Q436" s="37"/>
-      <c r="R436" s="37"/>
-      <c r="S436" s="37"/>
-      <c r="T436" s="37"/>
     </row>
     <row r="437" spans="1:20" ht="13" customHeight="1">
       <c r="A437" s="31"/>
@@ -13870,22 +13866,6 @@
       <c r="M544" s="28"/>
       <c r="N544" s="25"/>
     </row>
-    <row r="545" spans="1:14" ht="13" customHeight="1">
-      <c r="A545" s="31"/>
-      <c r="B545" s="27"/>
-      <c r="C545" s="30"/>
-      <c r="D545" s="27"/>
-      <c r="E545" s="27"/>
-      <c r="F545" s="27"/>
-      <c r="G545" s="27"/>
-      <c r="H545" s="27"/>
-      <c r="I545" s="27"/>
-      <c r="J545" s="27"/>
-      <c r="K545" s="27"/>
-      <c r="L545" s="27"/>
-      <c r="M545" s="28"/>
-      <c r="N545" s="25"/>
-    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -13893,7 +13873,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" xWindow="235" yWindow="427" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="235" yWindow="427" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Wertebereich!$G$2:$G$3</xm:f>

</xml_diff>

<commit_message>
Rename label and values of the privacy layer field.
To avoid problems with older repository excel configuration files, we
support both values (old and new).

No migration necessary, because only labels but no values changing.
</commit_message>
<xml_diff>
--- a/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/ordnungssystem.xlsx
+++ b/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/ordnungssystem.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flipsi/projects/opengever/2018/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flipsi/projects/opengever/2019/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB5D7E7-D51E-4943-9C40-02F73DBC12BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordnungssystem" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <definedNames>
     <definedName name="repository" localSheetId="0">Ordnungssystem!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,8 +32,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="repository.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="repository.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:lukas:Downloads:repository.csv" thousands="'" comma="1">
       <textFields count="24">
         <textField/>
@@ -146,12 +147,6 @@
     <t>Vertraulich</t>
   </si>
   <si>
-    <t>Keine Datenschutzstufe</t>
-  </si>
-  <si>
-    <t>Enthält schützenswerte Personendaten</t>
-  </si>
-  <si>
     <t>Nicht geprüft</t>
   </si>
   <si>
@@ -195,9 +190,6 @@
   <si>
     <t>Dossiers
 reaktivieren</t>
-  </si>
-  <si>
-    <t>Datenschutzstufe</t>
   </si>
   <si>
     <t>Archiv-
@@ -1057,11 +1049,20 @@
   <si>
     <t>lukas.graf, philippe.gross</t>
   </si>
+  <si>
+    <t>Datenschutz</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
@@ -1605,142 +1606,142 @@
     </xf>
   </cellXfs>
   <cellStyles count="136">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="134" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="19" builtinId="28"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2076,15 +2077,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Blatt1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Blatt1"/>
   <dimension ref="A1:T544"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="O18" sqref="O18"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2139,37 +2140,37 @@
     </row>
     <row r="3" spans="1:20" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>41</v>
+        <v>301</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>21</v>
@@ -2178,87 +2179,87 @@
         <v>22</v>
       </c>
       <c r="N3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="T3" s="9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="13" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="H4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="11" t="s">
+      <c r="J4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="L4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="11" t="s">
+      <c r="O4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="R4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="S4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="Q4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>55</v>
-      </c>
       <c r="T4" s="11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="50" customFormat="1" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2269,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>2</v>
@@ -2320,10 +2321,10 @@
         <v>17</v>
       </c>
       <c r="T5" s="51" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.15">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="20"/>
       <c r="B6" s="21" t="s">
         <v>18</v>
@@ -2353,13 +2354,13 @@
     </row>
     <row r="7" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="25" t="s">
@@ -2377,13 +2378,13 @@
     </row>
     <row r="8" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="25" t="s">
@@ -2401,13 +2402,13 @@
     </row>
     <row r="9" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="25" t="s">
@@ -2425,13 +2426,13 @@
     </row>
     <row r="10" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="25" t="s">
@@ -2440,34 +2441,34 @@
       <c r="L10" s="26"/>
       <c r="M10" s="23"/>
       <c r="N10" s="27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="P10" s="27" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="Q10" s="27" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="R10" s="27" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="S10" s="27" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="T10" s="27"/>
     </row>
     <row r="11" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="25" t="s">
@@ -2485,13 +2486,13 @@
     </row>
     <row r="12" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="25" t="s">
@@ -2509,16 +2510,16 @@
     </row>
     <row r="13" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>24</v>
@@ -2535,16 +2536,16 @@
     </row>
     <row r="14" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>24</v>
@@ -2553,10 +2554,10 @@
         <v>10</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L14" s="26"/>
       <c r="M14" s="23"/>
@@ -2570,13 +2571,13 @@
     </row>
     <row r="15" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="25" t="s">
@@ -2586,10 +2587,10 @@
         <v>10</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L15" s="26"/>
       <c r="M15" s="23"/>
@@ -2603,13 +2604,13 @@
     </row>
     <row r="16" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="25" t="s">
@@ -2619,10 +2620,10 @@
         <v>10</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L16" s="26"/>
       <c r="M16" s="23"/>
@@ -2636,16 +2637,16 @@
     </row>
     <row r="17" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>24</v>
@@ -2662,16 +2663,16 @@
     </row>
     <row r="18" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>24</v>
@@ -2680,31 +2681,31 @@
       <c r="M18" s="23"/>
       <c r="N18" s="27"/>
       <c r="O18" s="27" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="P18" s="27" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="Q18" s="27" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="R18" s="27" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="S18" s="27" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="T18" s="27"/>
     </row>
     <row r="19" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="25" t="s">
@@ -2722,13 +2723,13 @@
     </row>
     <row r="20" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="25" t="s">
@@ -2738,10 +2739,10 @@
         <v>10</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L20" s="26"/>
       <c r="M20" s="23"/>
@@ -2755,13 +2756,13 @@
     </row>
     <row r="21" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="25" t="s">
@@ -2771,10 +2772,10 @@
         <v>10</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L21" s="26"/>
       <c r="M21" s="23"/>
@@ -2788,13 +2789,13 @@
     </row>
     <row r="22" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="25" t="s">
@@ -2804,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L22" s="26"/>
       <c r="M22" s="23"/>
@@ -2821,13 +2822,13 @@
     </row>
     <row r="23" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="25" t="s">
@@ -2845,13 +2846,13 @@
     </row>
     <row r="24" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="25" t="s">
@@ -2861,10 +2862,10 @@
         <v>10</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L24" s="26"/>
       <c r="M24" s="23"/>
@@ -2878,13 +2879,13 @@
     </row>
     <row r="25" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="25" t="s">
@@ -2894,10 +2895,10 @@
         <v>10</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L25" s="26"/>
       <c r="M25" s="23"/>
@@ -2911,13 +2912,13 @@
     </row>
     <row r="26" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="25" t="s">
@@ -2927,10 +2928,10 @@
         <v>10</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L26" s="26"/>
       <c r="M26" s="23"/>
@@ -2944,13 +2945,13 @@
     </row>
     <row r="27" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="25" t="s">
@@ -2968,13 +2969,13 @@
     </row>
     <row r="28" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="25" t="s">
@@ -2992,13 +2993,13 @@
     </row>
     <row r="29" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="25" t="s">
@@ -3008,10 +3009,10 @@
         <v>10</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L29" s="26"/>
       <c r="M29" s="23"/>
@@ -3025,13 +3026,13 @@
     </row>
     <row r="30" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="25" t="s">
@@ -3049,13 +3050,13 @@
     </row>
     <row r="31" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="25" t="s">
@@ -3073,13 +3074,13 @@
     </row>
     <row r="32" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="25" t="s">
@@ -3089,10 +3090,10 @@
         <v>10</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L32" s="26"/>
       <c r="M32" s="23"/>
@@ -3106,13 +3107,13 @@
     </row>
     <row r="33" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="25" t="s">
@@ -3130,13 +3131,13 @@
     </row>
     <row r="34" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="25" t="s">
@@ -3154,13 +3155,13 @@
     </row>
     <row r="35" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="25" t="s">
@@ -3178,13 +3179,13 @@
     </row>
     <row r="36" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="25" t="s">
@@ -3202,16 +3203,16 @@
     </row>
     <row r="37" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>24</v>
@@ -3228,13 +3229,13 @@
     </row>
     <row r="38" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="25" t="s">
@@ -3252,13 +3253,13 @@
     </row>
     <row r="39" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="25" t="s">
@@ -3276,13 +3277,13 @@
     </row>
     <row r="40" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="25" t="s">
@@ -3300,13 +3301,13 @@
     </row>
     <row r="41" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D41" s="19"/>
       <c r="E41" s="25" t="s">
@@ -3324,13 +3325,13 @@
     </row>
     <row r="42" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="25" t="s">
@@ -3348,13 +3349,13 @@
     </row>
     <row r="43" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="25" t="s">
@@ -3372,13 +3373,13 @@
     </row>
     <row r="44" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="25" t="s">
@@ -3396,13 +3397,13 @@
     </row>
     <row r="45" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="25" t="s">
@@ -3420,13 +3421,13 @@
     </row>
     <row r="46" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="25" t="s">
@@ -3436,10 +3437,10 @@
         <v>10</v>
       </c>
       <c r="H46" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I46" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L46" s="26"/>
       <c r="M46" s="23"/>
@@ -3453,13 +3454,13 @@
     </row>
     <row r="47" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="25" t="s">
@@ -3477,13 +3478,13 @@
     </row>
     <row r="48" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="25" t="s">
@@ -3493,10 +3494,10 @@
         <v>25</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I48" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L48" s="26"/>
       <c r="M48" s="23"/>
@@ -3510,13 +3511,13 @@
     </row>
     <row r="49" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="25" t="s">
@@ -3526,10 +3527,10 @@
         <v>10</v>
       </c>
       <c r="H49" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I49" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L49" s="26"/>
       <c r="M49" s="23"/>
@@ -3543,16 +3544,16 @@
     </row>
     <row r="50" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E50" s="25" t="s">
         <v>24</v>
@@ -3561,10 +3562,10 @@
         <v>25</v>
       </c>
       <c r="H50" s="25" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I50" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L50" s="26"/>
       <c r="M50" s="23"/>
@@ -3578,13 +3579,13 @@
     </row>
     <row r="51" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="25" t="s">
@@ -3594,10 +3595,10 @@
         <v>25</v>
       </c>
       <c r="H51" s="25" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I51" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L51" s="26"/>
       <c r="M51" s="23"/>
@@ -3611,13 +3612,13 @@
     </row>
     <row r="52" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="17" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D52" s="19"/>
       <c r="E52" s="25" t="s">
@@ -3635,13 +3636,13 @@
     </row>
     <row r="53" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="25" t="s">
@@ -3659,13 +3660,13 @@
     </row>
     <row r="54" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="17" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D54" s="19"/>
       <c r="E54" s="25" t="s">
@@ -3675,10 +3676,10 @@
         <v>10</v>
       </c>
       <c r="H54" s="25" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I54" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L54" s="26"/>
       <c r="M54" s="23"/>
@@ -3692,16 +3693,16 @@
     </row>
     <row r="55" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E55" s="25" t="s">
         <v>24</v>
@@ -3710,10 +3711,10 @@
         <v>10</v>
       </c>
       <c r="H55" s="25" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="I55" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L55" s="26"/>
       <c r="M55" s="23"/>
@@ -3727,13 +3728,13 @@
     </row>
     <row r="56" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="17" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D56" s="19"/>
       <c r="E56" s="25" t="s">
@@ -3743,10 +3744,10 @@
         <v>10</v>
       </c>
       <c r="H56" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I56" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L56" s="26"/>
       <c r="M56" s="23"/>
@@ -3760,13 +3761,13 @@
     </row>
     <row r="57" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D57" s="19"/>
       <c r="E57" s="25" t="s">
@@ -3776,10 +3777,10 @@
         <v>25</v>
       </c>
       <c r="H57" s="25" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="I57" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L57" s="26"/>
       <c r="M57" s="23"/>
@@ -3793,13 +3794,13 @@
     </row>
     <row r="58" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="17" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D58" s="19"/>
       <c r="E58" s="25" t="s">
@@ -3817,13 +3818,13 @@
     </row>
     <row r="59" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D59" s="19"/>
       <c r="E59" s="25" t="s">
@@ -3841,16 +3842,16 @@
     </row>
     <row r="60" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="17" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D60" s="19" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E60" s="25" t="s">
         <v>24</v>
@@ -3859,10 +3860,10 @@
         <v>10</v>
       </c>
       <c r="H60" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I60" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L60" s="26"/>
       <c r="M60" s="23"/>
@@ -3876,13 +3877,13 @@
     </row>
     <row r="61" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="17" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D61" s="19"/>
       <c r="E61" s="25" t="s">
@@ -3892,10 +3893,10 @@
         <v>10</v>
       </c>
       <c r="H61" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I61" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L61" s="26"/>
       <c r="M61" s="23"/>
@@ -3909,13 +3910,13 @@
     </row>
     <row r="62" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="17" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D62" s="19"/>
       <c r="E62" s="25" t="s">
@@ -3933,16 +3934,16 @@
     </row>
     <row r="63" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="17" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E63" s="25" t="s">
         <v>24</v>
@@ -3951,10 +3952,10 @@
         <v>10</v>
       </c>
       <c r="H63" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I63" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L63" s="26"/>
       <c r="M63" s="23"/>
@@ -3968,16 +3969,16 @@
     </row>
     <row r="64" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="17" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E64" s="25" t="s">
         <v>24</v>
@@ -3986,10 +3987,10 @@
         <v>10</v>
       </c>
       <c r="H64" s="25" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="I64" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L64" s="26"/>
       <c r="M64" s="23"/>
@@ -4003,16 +4004,16 @@
     </row>
     <row r="65" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="17" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D65" s="19" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E65" s="25" t="s">
         <v>24</v>
@@ -4021,10 +4022,10 @@
         <v>10</v>
       </c>
       <c r="H65" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I65" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L65" s="26"/>
       <c r="M65" s="23"/>
@@ -4038,16 +4039,16 @@
     </row>
     <row r="66" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="17" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D66" s="19" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E66" s="25" t="s">
         <v>24</v>
@@ -4056,10 +4057,10 @@
         <v>10</v>
       </c>
       <c r="H66" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I66" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L66" s="26"/>
       <c r="M66" s="23"/>
@@ -4073,16 +4074,16 @@
     </row>
     <row r="67" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E67" s="25" t="s">
         <v>24</v>
@@ -4091,10 +4092,10 @@
         <v>10</v>
       </c>
       <c r="H67" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I67" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L67" s="26"/>
       <c r="M67" s="23"/>
@@ -4108,13 +4109,13 @@
     </row>
     <row r="68" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D68" s="19"/>
       <c r="E68" s="25" t="s">
@@ -4124,10 +4125,10 @@
         <v>10</v>
       </c>
       <c r="H68" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I68" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L68" s="26"/>
       <c r="M68" s="23"/>
@@ -4141,16 +4142,16 @@
     </row>
     <row r="69" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E69" s="25" t="s">
         <v>24</v>
@@ -4159,10 +4160,10 @@
         <v>10</v>
       </c>
       <c r="H69" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I69" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L69" s="26"/>
       <c r="M69" s="23"/>
@@ -4176,13 +4177,13 @@
     </row>
     <row r="70" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D70" s="19"/>
       <c r="E70" s="25" t="s">
@@ -4200,13 +4201,13 @@
     </row>
     <row r="71" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D71" s="19"/>
       <c r="E71" s="25" t="s">
@@ -4224,13 +4225,13 @@
     </row>
     <row r="72" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="17" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D72" s="19"/>
       <c r="E72" s="25" t="s">
@@ -4248,13 +4249,13 @@
     </row>
     <row r="73" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D73" s="19"/>
       <c r="E73" s="25" t="s">
@@ -4272,13 +4273,13 @@
     </row>
     <row r="74" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D74" s="19"/>
       <c r="E74" s="25" t="s">
@@ -4288,10 +4289,10 @@
         <v>10</v>
       </c>
       <c r="H74" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I74" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L74" s="26"/>
       <c r="M74" s="23"/>
@@ -4305,16 +4306,16 @@
     </row>
     <row r="75" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="17" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D75" s="19" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E75" s="25" t="s">
         <v>24</v>
@@ -4323,10 +4324,10 @@
         <v>10</v>
       </c>
       <c r="H75" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I75" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L75" s="26"/>
       <c r="M75" s="23"/>
@@ -4340,16 +4341,16 @@
     </row>
     <row r="76" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D76" s="19" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E76" s="25" t="s">
         <v>24</v>
@@ -4358,10 +4359,10 @@
         <v>10</v>
       </c>
       <c r="H76" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I76" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L76" s="26"/>
       <c r="M76" s="23"/>
@@ -4375,13 +4376,13 @@
     </row>
     <row r="77" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="17" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D77" s="19"/>
       <c r="E77" s="25" t="s">
@@ -4391,10 +4392,10 @@
         <v>10</v>
       </c>
       <c r="H77" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I77" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L77" s="26"/>
       <c r="M77" s="23"/>
@@ -4408,16 +4409,16 @@
     </row>
     <row r="78" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D78" s="19" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E78" s="25" t="s">
         <v>24</v>
@@ -4426,10 +4427,10 @@
         <v>10</v>
       </c>
       <c r="H78" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I78" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L78" s="26"/>
       <c r="M78" s="23"/>
@@ -4443,13 +4444,13 @@
     </row>
     <row r="79" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D79" s="19"/>
       <c r="E79" s="25" t="s">
@@ -4470,13 +4471,13 @@
     </row>
     <row r="80" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="17" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D80" s="19"/>
       <c r="E80" s="25" t="s">
@@ -4486,10 +4487,10 @@
         <v>10</v>
       </c>
       <c r="H80" s="25" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I80" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L80" s="26"/>
       <c r="M80" s="23"/>
@@ -4503,13 +4504,13 @@
     </row>
     <row r="81" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D81" s="19"/>
       <c r="E81" s="25" t="s">
@@ -4527,13 +4528,13 @@
     </row>
     <row r="82" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="17" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D82" s="19"/>
       <c r="E82" s="25" t="s">
@@ -13859,37 +13860,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="235" yWindow="427" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Wertebereich!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>F7:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Wertebereich!$O$2:$O$4</xm:f>
           </x14:formula1>
           <xm:sqref>N7:N1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Wertebereich!$F$2:$F$4</xm:f>
           </x14:formula1>
           <xm:sqref>E7:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Wertebereich!$J$2:$J$7</xm:f>
           </x14:formula1>
           <xm:sqref>I7:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>Wertebereich!$H$2:$H$6</xm:f>
           </x14:formula1>
           <xm:sqref>G7:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>Wertebereich!$L$2:$L$4</xm:f>
           </x14:formula1>
@@ -13902,12 +13903,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Blatt2" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Blatt2"/>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13981,7 +13982,7 @@
         <v>17</v>
       </c>
       <c r="U1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -13989,19 +13990,19 @@
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>302</v>
       </c>
       <c r="H2">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L2">
         <v>30</v>
       </c>
       <c r="O2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -14009,30 +14010,30 @@
         <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>303</v>
       </c>
       <c r="H3">
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4">
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L4">
         <v>150</v>
@@ -14043,7 +14044,7 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -14051,12 +14052,12 @@
         <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="J7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add space for repo root permissions in excel.
</commit_message>
<xml_diff>
--- a/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/ordnungssystem.xlsx
+++ b/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/ordnungssystem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flipsi/projects/opengever/2019/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deif/Files/workspaces/opengever.core/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB5D7E7-D51E-4943-9C40-02F73DBC12BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C042D99E-0463-4A45-B6E6-0ACFA28F6EE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordnungssystem" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="repository" localSheetId="0">Ordnungssystem!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="305">
   <si>
     <t>reference_number</t>
   </si>
@@ -1057,6 +1057,9 @@
   </si>
   <si>
     <t>Nein</t>
+  </si>
+  <si>
+    <t>og_demo-ftw_users</t>
   </si>
 </sst>
 </file>
@@ -1441,7 +1444,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1604,144 +1607,145 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="136">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="24" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="26" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="28" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="30" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="32" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="34" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="36" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="38" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="40" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="72" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="74" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="76" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="78" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="80" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="82" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="84" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="86" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="88" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="90" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="92" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="19" builtinId="28"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2082,10 +2086,10 @@
   <dimension ref="A1:T544"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2345,12 +2349,24 @@
         <v>73050</v>
       </c>
       <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
+      <c r="O6" s="53" t="s">
+        <v>304</v>
+      </c>
+      <c r="P6" s="53" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q6" s="53" t="s">
+        <v>304</v>
+      </c>
+      <c r="R6" s="53" t="s">
+        <v>304</v>
+      </c>
+      <c r="S6" s="53" t="s">
+        <v>304</v>
+      </c>
+      <c r="T6" s="53" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="7" spans="1:20" s="25" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52" t="s">

</xml_diff>